<commit_message>
Updated code to use relative paths + added Excel summary files
</commit_message>
<xml_diff>
--- a/Branch_Summary.xlsx
+++ b/Branch_Summary.xlsx
@@ -814,25 +814,25 @@
         <v>45922</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02686528310020379</v>
+        <v>0.02565433749903027</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01390973851663206</v>
+        <v>0.01371997570982115</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.01295554458357173</v>
+        <v>-0.01193436178920912</v>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L9" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -898,25 +898,25 @@
         <v>45922</v>
       </c>
       <c r="F11" t="n">
-        <v>0.03907570933158688</v>
+        <v>0.03714633195887534</v>
       </c>
       <c r="G11" t="n">
-        <v>0.02507134882070972</v>
+        <v>0.02502407388697692</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.01400436051087715</v>
+        <v>-0.01212225807189842</v>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L11" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -1024,25 +1024,25 @@
         <v>45922</v>
       </c>
       <c r="F14" t="n">
-        <v>0.03688715953307393</v>
+        <v>0.03593121156752885</v>
       </c>
       <c r="G14" t="n">
-        <v>0.02320744028063787</v>
+        <v>0.02267446416838272</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.01367971925243607</v>
+        <v>-0.01325674739914613</v>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L14" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -1279,10 +1279,10 @@
         <v>0.03678776629845384</v>
       </c>
       <c r="G20" t="n">
-        <v>0.028719806109983</v>
+        <v>0.02879381107269849</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.008067960188470846</v>
+        <v>-0.007993955225755359</v>
       </c>
       <c r="I20" t="n">
         <v>5</v>
@@ -1294,7 +1294,7 @@
         <v>30</v>
       </c>
       <c r="L20" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
@@ -1363,10 +1363,10 @@
         <v>0.05505057800021645</v>
       </c>
       <c r="G22" t="n">
-        <v>0.03914254156214057</v>
+        <v>0.03956253439534069</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.01590803643807588</v>
+        <v>-0.01548804360487576</v>
       </c>
       <c r="I22" t="n">
         <v>5</v>
@@ -1378,7 +1378,7 @@
         <v>19</v>
       </c>
       <c r="L22" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
@@ -1447,10 +1447,10 @@
         <v>0.06438316930807703</v>
       </c>
       <c r="G24" t="n">
-        <v>0.04725696006021556</v>
+        <v>0.04745412022106114</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.01712620924786146</v>
+        <v>-0.01692904908701588</v>
       </c>
       <c r="I24" t="n">
         <v>5</v>
@@ -1462,7 +1462,7 @@
         <v>18</v>
       </c>
       <c r="L24" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25">
@@ -1486,25 +1486,25 @@
         <v>45922</v>
       </c>
       <c r="F25" t="n">
-        <v>0.05851703406813628</v>
+        <v>0.05686372745490982</v>
       </c>
       <c r="G25" t="n">
-        <v>0.03663072111965868</v>
+        <v>0.0373488913310492</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.0218863129484776</v>
+        <v>-0.01951483612386062</v>
       </c>
       <c r="I25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K25" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L25" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -1654,25 +1654,25 @@
         <v>45922</v>
       </c>
       <c r="F29" t="n">
-        <v>0.04597701149425287</v>
+        <v>0.04499178981937602</v>
       </c>
       <c r="G29" t="n">
-        <v>0.02442571134634648</v>
+        <v>0.02404476992356354</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.02155130014790639</v>
+        <v>-0.02094701989581248</v>
       </c>
       <c r="I29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K29" t="n">
+        <v>7</v>
+      </c>
+      <c r="L29" t="n">
         <v>6</v>
-      </c>
-      <c r="L29" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="30">
@@ -1822,25 +1822,25 @@
         <v>45922</v>
       </c>
       <c r="F33" t="n">
-        <v>0.04559874927538778</v>
+        <v>0.04527409000462209</v>
       </c>
       <c r="G33" t="n">
-        <v>0.03223249669749009</v>
+        <v>0.03206359939471828</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.01336625257789768</v>
+        <v>-0.01321049060990381</v>
       </c>
       <c r="I33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K33" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L33" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
@@ -1948,25 +1948,25 @@
         <v>45922</v>
       </c>
       <c r="F36" t="n">
-        <v>0.07933042212518196</v>
+        <v>0.0771823805421524</v>
       </c>
       <c r="G36" t="n">
-        <v>0.05024495092406808</v>
+        <v>0.04995933136849945</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.02908547120111388</v>
+        <v>-0.02722304917365295</v>
       </c>
       <c r="I36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K36" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L36" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
@@ -2074,13 +2074,13 @@
         <v>45917</v>
       </c>
       <c r="F39" t="n">
-        <v>0.06459804799606625</v>
+        <v>0.06459804799606626</v>
       </c>
       <c r="G39" t="n">
-        <v>0.04816622911636468</v>
+        <v>0.04842936568888473</v>
       </c>
       <c r="H39" t="n">
-        <v>-0.01643181887970157</v>
+        <v>-0.01616868230718153</v>
       </c>
       <c r="I39" t="n">
         <v>5</v>
@@ -2092,7 +2092,7 @@
         <v>18</v>
       </c>
       <c r="L39" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40">
@@ -2203,10 +2203,10 @@
         <v>0.04550441790933918</v>
       </c>
       <c r="G42" t="n">
-        <v>0.0338721207034674</v>
+        <v>0.03367003291278636</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.01163229720587178</v>
+        <v>-0.01183438499655282</v>
       </c>
       <c r="I42" t="n">
         <v>5</v>
@@ -2218,7 +2218,7 @@
         <v>25</v>
       </c>
       <c r="L42" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43">
@@ -2245,10 +2245,10 @@
         <v>0.05564191901889028</v>
       </c>
       <c r="G43" t="n">
-        <v>0.03500844310056654</v>
+        <v>0.03531661849741008</v>
       </c>
       <c r="H43" t="n">
-        <v>-0.02063347591832374</v>
+        <v>-0.0203253005214802</v>
       </c>
       <c r="I43" t="n">
         <v>5</v>
@@ -2260,7 +2260,7 @@
         <v>12</v>
       </c>
       <c r="L43" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44">
@@ -2371,10 +2371,10 @@
         <v>0.03603663064103622</v>
       </c>
       <c r="G46" t="n">
-        <v>0.02995603126739467</v>
+        <v>0.03009155778372049</v>
       </c>
       <c r="H46" t="n">
-        <v>-0.006080599373641547</v>
+        <v>-0.005945072857315725</v>
       </c>
       <c r="I46" t="n">
         <v>5</v>
@@ -2386,7 +2386,7 @@
         <v>18</v>
       </c>
       <c r="L46" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47">
@@ -2416,7 +2416,7 @@
         <v>0.01935889956319769</v>
       </c>
       <c r="H47" t="n">
-        <v>-0.009556983395204194</v>
+        <v>-0.00955698339520419</v>
       </c>
       <c r="I47" t="n">
         <v>5</v>
@@ -2497,10 +2497,10 @@
         <v>0.06150674523410282</v>
       </c>
       <c r="G49" t="n">
-        <v>0.04021565255174909</v>
+        <v>0.04071384221759424</v>
       </c>
       <c r="H49" t="n">
-        <v>-0.02129109268235373</v>
+        <v>-0.02079290301650858</v>
       </c>
       <c r="I49" t="n">
         <v>5</v>
@@ -2512,7 +2512,7 @@
         <v>13</v>
       </c>
       <c r="L49" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -2665,10 +2665,10 @@
         <v>0.04252181736692828</v>
       </c>
       <c r="G53" t="n">
-        <v>0.02588352032776106</v>
+        <v>0.02598346064312904</v>
       </c>
       <c r="H53" t="n">
-        <v>-0.01663829703916722</v>
+        <v>-0.01653835672379925</v>
       </c>
       <c r="I53" t="n">
         <v>5</v>
@@ -2680,7 +2680,7 @@
         <v>17</v>
       </c>
       <c r="L53" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54">
@@ -2749,10 +2749,10 @@
         <v>0.03982025059266728</v>
       </c>
       <c r="G55" t="n">
-        <v>0.02798270192328202</v>
+        <v>0.02791311760325681</v>
       </c>
       <c r="H55" t="n">
-        <v>-0.01183754866938527</v>
+        <v>-0.01190713298941047</v>
       </c>
       <c r="I55" t="n">
         <v>5</v>
@@ -2764,7 +2764,7 @@
         <v>22</v>
       </c>
       <c r="L55" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56">
@@ -2830,13 +2830,13 @@
         <v>45917</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0413040869190424</v>
+        <v>0.04130408691904243</v>
       </c>
       <c r="G57" t="n">
-        <v>0.02487940808946815</v>
+        <v>0.02487940808946816</v>
       </c>
       <c r="H57" t="n">
-        <v>-0.01642467882957425</v>
+        <v>-0.01642467882957427</v>
       </c>
       <c r="I57" t="n">
         <v>5</v>
@@ -2872,13 +2872,13 @@
         <v>45917</v>
       </c>
       <c r="F58" t="n">
-        <v>0.0407108198057396</v>
+        <v>0.04071081980573961</v>
       </c>
       <c r="G58" t="n">
-        <v>0.03780645107030316</v>
+        <v>0.03780645107030312</v>
       </c>
       <c r="H58" t="n">
-        <v>-0.002904368735436445</v>
+        <v>-0.002904368735436487</v>
       </c>
       <c r="I58" t="n">
         <v>5</v>
@@ -2914,13 +2914,13 @@
         <v>45917</v>
       </c>
       <c r="F59" t="n">
-        <v>0.03075035865036883</v>
+        <v>0.03075035865036881</v>
       </c>
       <c r="G59" t="n">
-        <v>0.02575516547841619</v>
+        <v>0.02575516547841616</v>
       </c>
       <c r="H59" t="n">
-        <v>-0.004995193171952645</v>
+        <v>-0.004995193171952642</v>
       </c>
       <c r="I59" t="n">
         <v>5</v>
@@ -2956,10 +2956,10 @@
         <v>45917</v>
       </c>
       <c r="F60" t="n">
-        <v>0.02944555495008482</v>
+        <v>0.02944555495008478</v>
       </c>
       <c r="G60" t="n">
-        <v>0.02596343999073791</v>
+        <v>0.02596343999073788</v>
       </c>
       <c r="H60" t="n">
         <v>-0.003482114959346905</v>
@@ -2998,13 +2998,13 @@
         <v>45917</v>
       </c>
       <c r="F61" t="n">
-        <v>0.05127540802356448</v>
+        <v>0.05127540802356442</v>
       </c>
       <c r="G61" t="n">
-        <v>0.0400104762111602</v>
+        <v>0.04001047621116013</v>
       </c>
       <c r="H61" t="n">
-        <v>-0.01126493181240427</v>
+        <v>-0.0112649318124043</v>
       </c>
       <c r="I61" t="n">
         <v>5</v>
@@ -3040,13 +3040,13 @@
         <v>45917</v>
       </c>
       <c r="F62" t="n">
-        <v>0.05475800446464329</v>
+        <v>0.05475800446464337</v>
       </c>
       <c r="G62" t="n">
-        <v>0.03296745623266348</v>
+        <v>0.0329674562326635</v>
       </c>
       <c r="H62" t="n">
-        <v>-0.0217905482319798</v>
+        <v>-0.02179054823197987</v>
       </c>
       <c r="I62" t="n">
         <v>5</v>
@@ -3082,13 +3082,13 @@
         <v>45917</v>
       </c>
       <c r="F63" t="n">
-        <v>0.04168202642261191</v>
+        <v>0.04168202642261185</v>
       </c>
       <c r="G63" t="n">
-        <v>0.02633361110123002</v>
+        <v>0.02633361110123</v>
       </c>
       <c r="H63" t="n">
-        <v>-0.01534841532138189</v>
+        <v>-0.01534841532138185</v>
       </c>
       <c r="I63" t="n">
         <v>5</v>
@@ -3124,25 +3124,25 @@
         <v>45922</v>
       </c>
       <c r="F64" t="n">
-        <v>0.02409821382664498</v>
+        <v>0.02293850550752172</v>
       </c>
       <c r="G64" t="n">
-        <v>0.0122031830493839</v>
+        <v>0.01193126250668339</v>
       </c>
       <c r="H64" t="n">
-        <v>-0.01189503077726109</v>
+        <v>-0.01100724300083833</v>
       </c>
       <c r="I64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K64" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L64" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65">
@@ -3166,13 +3166,13 @@
         <v>45917</v>
       </c>
       <c r="F65" t="n">
-        <v>0.038713417590166</v>
+        <v>0.03871341759016594</v>
       </c>
       <c r="G65" t="n">
-        <v>0.02602035247543372</v>
+        <v>0.02602035247543365</v>
       </c>
       <c r="H65" t="n">
-        <v>-0.01269306511473228</v>
+        <v>-0.0126930651147323</v>
       </c>
       <c r="I65" t="n">
         <v>5</v>
@@ -3208,25 +3208,25 @@
         <v>45922</v>
       </c>
       <c r="F66" t="n">
-        <v>0.03734079211551622</v>
+        <v>0.03619723639204042</v>
       </c>
       <c r="G66" t="n">
-        <v>0.02400177941195379</v>
+        <v>0.0240414770224144</v>
       </c>
       <c r="H66" t="n">
-        <v>-0.01333901270356243</v>
+        <v>-0.01215575936962602</v>
       </c>
       <c r="I66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K66" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L66" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67">
@@ -3250,13 +3250,13 @@
         <v>45917</v>
       </c>
       <c r="F67" t="n">
-        <v>0.04264159283682144</v>
+        <v>0.04264159283682149</v>
       </c>
       <c r="G67" t="n">
-        <v>0.03017137449870454</v>
+        <v>0.03017137449870455</v>
       </c>
       <c r="H67" t="n">
-        <v>-0.0124702183381169</v>
+        <v>-0.01247021833811694</v>
       </c>
       <c r="I67" t="n">
         <v>5</v>
@@ -3292,13 +3292,13 @@
         <v>45917</v>
       </c>
       <c r="F68" t="n">
-        <v>0.03201386543828729</v>
+        <v>0.03201386543828737</v>
       </c>
       <c r="G68" t="n">
-        <v>0.02397689721615975</v>
+        <v>0.02397689721615979</v>
       </c>
       <c r="H68" t="n">
-        <v>-0.008036968222127537</v>
+        <v>-0.008036968222127582</v>
       </c>
       <c r="I68" t="n">
         <v>5</v>
@@ -3334,25 +3334,25 @@
         <v>45922</v>
       </c>
       <c r="F69" t="n">
-        <v>0.03885588576456642</v>
+        <v>0.03601474986643606</v>
       </c>
       <c r="G69" t="n">
-        <v>0.01717928611055422</v>
+        <v>0.01637877035211194</v>
       </c>
       <c r="H69" t="n">
-        <v>-0.0216765996540122</v>
+        <v>-0.01963597951432412</v>
       </c>
       <c r="I69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K69" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L69" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70">
@@ -3382,7 +3382,7 @@
         <v>0.07676459848976826</v>
       </c>
       <c r="H70" t="n">
-        <v>-0.0244583397735349</v>
+        <v>-0.02445833977353498</v>
       </c>
       <c r="I70" t="n">
         <v>5</v>
@@ -3418,13 +3418,13 @@
         <v>45917</v>
       </c>
       <c r="F71" t="n">
-        <v>0.06151431706147018</v>
+        <v>0.06151431706147027</v>
       </c>
       <c r="G71" t="n">
-        <v>0.04345434321970936</v>
+        <v>0.04345434321970942</v>
       </c>
       <c r="H71" t="n">
-        <v>-0.01805997384176082</v>
+        <v>-0.01805997384176086</v>
       </c>
       <c r="I71" t="n">
         <v>5</v>
@@ -3463,10 +3463,10 @@
         <v>0.06699982531517511</v>
       </c>
       <c r="G72" t="n">
-        <v>0.05147302997515824</v>
+        <v>0.05147302997515826</v>
       </c>
       <c r="H72" t="n">
-        <v>-0.01552679534001686</v>
+        <v>-0.01552679534001685</v>
       </c>
       <c r="I72" t="n">
         <v>5</v>
@@ -3544,13 +3544,13 @@
         <v>45917</v>
       </c>
       <c r="F74" t="n">
-        <v>0.04016968427979487</v>
+        <v>0.04016968427979491</v>
       </c>
       <c r="G74" t="n">
-        <v>0.03014017509027051</v>
+        <v>0.03014017509027054</v>
       </c>
       <c r="H74" t="n">
-        <v>-0.01002950918952436</v>
+        <v>-0.01002950918952437</v>
       </c>
       <c r="I74" t="n">
         <v>5</v>
@@ -3586,13 +3586,13 @@
         <v>45917</v>
       </c>
       <c r="F75" t="n">
-        <v>0.0401294808802416</v>
+        <v>0.04012948088024149</v>
       </c>
       <c r="G75" t="n">
-        <v>0.02937307095685369</v>
+        <v>0.02947369788387295</v>
       </c>
       <c r="H75" t="n">
-        <v>-0.01075640992338791</v>
+        <v>-0.01065578299636855</v>
       </c>
       <c r="I75" t="n">
         <v>5</v>
@@ -3604,7 +3604,7 @@
         <v>30</v>
       </c>
       <c r="L75" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76">
@@ -3628,13 +3628,13 @@
         <v>45917</v>
       </c>
       <c r="F76" t="n">
-        <v>0.02236715386841787</v>
+        <v>0.02236715386841782</v>
       </c>
       <c r="G76" t="n">
-        <v>0.01709844969182691</v>
+        <v>0.01709844969182687</v>
       </c>
       <c r="H76" t="n">
-        <v>-0.005268704176590963</v>
+        <v>-0.005268704176590956</v>
       </c>
       <c r="I76" t="n">
         <v>5</v>
@@ -3670,13 +3670,13 @@
         <v>45917</v>
       </c>
       <c r="F77" t="n">
-        <v>0.04900708354631916</v>
+        <v>0.04900708354631914</v>
       </c>
       <c r="G77" t="n">
-        <v>0.0328652454490169</v>
+        <v>0.03310556277797057</v>
       </c>
       <c r="H77" t="n">
-        <v>-0.01614183809730226</v>
+        <v>-0.01590152076834857</v>
       </c>
       <c r="I77" t="n">
         <v>5</v>
@@ -3688,7 +3688,7 @@
         <v>19</v>
       </c>
       <c r="L77" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78">
@@ -3712,13 +3712,13 @@
         <v>45917</v>
       </c>
       <c r="F78" t="n">
-        <v>0.02494092426637897</v>
+        <v>0.02494092426637896</v>
       </c>
       <c r="G78" t="n">
         <v>0.01829591920289108</v>
       </c>
       <c r="H78" t="n">
-        <v>-0.006645005063487891</v>
+        <v>-0.006645005063487877</v>
       </c>
       <c r="I78" t="n">
         <v>5</v>
@@ -3754,13 +3754,13 @@
         <v>45917</v>
       </c>
       <c r="F79" t="n">
-        <v>0.07149785290719404</v>
+        <v>0.07149785290719401</v>
       </c>
       <c r="G79" t="n">
-        <v>0.05091037147490596</v>
+        <v>0.05127901084392853</v>
       </c>
       <c r="H79" t="n">
-        <v>-0.02058748143228808</v>
+        <v>-0.02021884206326548</v>
       </c>
       <c r="I79" t="n">
         <v>5</v>
@@ -3772,7 +3772,7 @@
         <v>18</v>
       </c>
       <c r="L79" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80">
@@ -3796,25 +3796,25 @@
         <v>45922</v>
       </c>
       <c r="F80" t="n">
-        <v>0.05284033289577121</v>
+        <v>0.05068900116102207</v>
       </c>
       <c r="G80" t="n">
-        <v>0.03346978938540853</v>
+        <v>0.03446776007468507</v>
       </c>
       <c r="H80" t="n">
-        <v>-0.01937054351036268</v>
+        <v>-0.016221241086337</v>
       </c>
       <c r="I80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K80" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L80" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81">
@@ -3838,13 +3838,13 @@
         <v>45917</v>
       </c>
       <c r="F81" t="n">
-        <v>0.04394437952640065</v>
+        <v>0.04394437952640063</v>
       </c>
       <c r="G81" t="n">
-        <v>0.03919247770352011</v>
+        <v>0.03919247770352008</v>
       </c>
       <c r="H81" t="n">
-        <v>-0.004751901822880544</v>
+        <v>-0.004751901822880551</v>
       </c>
       <c r="I81" t="n">
         <v>5</v>
@@ -3880,13 +3880,13 @@
         <v>45917</v>
       </c>
       <c r="F82" t="n">
-        <v>0.06919261166002105</v>
+        <v>0.06919261166002108</v>
       </c>
       <c r="G82" t="n">
-        <v>0.0415024159808836</v>
+        <v>0.04150241598088361</v>
       </c>
       <c r="H82" t="n">
-        <v>-0.02769019567913745</v>
+        <v>-0.02769019567913747</v>
       </c>
       <c r="I82" t="n">
         <v>5</v>
@@ -3925,10 +3925,10 @@
         <v>0.04524836021041063</v>
       </c>
       <c r="G83" t="n">
-        <v>0.03868839848143018</v>
+        <v>0.03868839848143017</v>
       </c>
       <c r="H83" t="n">
-        <v>-0.006559961728980448</v>
+        <v>-0.006559961728980462</v>
       </c>
       <c r="I83" t="n">
         <v>5</v>
@@ -3964,25 +3964,25 @@
         <v>45922</v>
       </c>
       <c r="F84" t="n">
-        <v>0.04806656149045466</v>
+        <v>0.04665844512236778</v>
       </c>
       <c r="G84" t="n">
-        <v>0.01969087328777141</v>
+        <v>0.01897672093791386</v>
       </c>
       <c r="H84" t="n">
-        <v>-0.02837568820268326</v>
+        <v>-0.02768172418445391</v>
       </c>
       <c r="I84" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J84" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K84" t="n">
+        <v>7</v>
+      </c>
+      <c r="L84" t="n">
         <v>6</v>
-      </c>
-      <c r="L84" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="85">
@@ -4006,13 +4006,13 @@
         <v>45917</v>
       </c>
       <c r="F85" t="n">
-        <v>0.03271367967651072</v>
+        <v>0.03271367967651074</v>
       </c>
       <c r="G85" t="n">
-        <v>0.02892274020882466</v>
+        <v>0.02892274020882468</v>
       </c>
       <c r="H85" t="n">
-        <v>-0.003790939467686067</v>
+        <v>-0.003790939467686064</v>
       </c>
       <c r="I85" t="n">
         <v>5</v>
@@ -4048,13 +4048,13 @@
         <v>45917</v>
       </c>
       <c r="F86" t="n">
-        <v>0.0833963828931031</v>
+        <v>0.08339638289310312</v>
       </c>
       <c r="G86" t="n">
         <v>0.07377830061061369</v>
       </c>
       <c r="H86" t="n">
-        <v>-0.009618082282489407</v>
+        <v>-0.009618082282489435</v>
       </c>
       <c r="I86" t="n">
         <v>5</v>
@@ -4090,13 +4090,13 @@
         <v>45917</v>
       </c>
       <c r="F87" t="n">
-        <v>0.06123215978813644</v>
+        <v>0.06123215978813642</v>
       </c>
       <c r="G87" t="n">
-        <v>0.04913965889576544</v>
+        <v>0.04913965889576541</v>
       </c>
       <c r="H87" t="n">
-        <v>-0.012092500892371</v>
+        <v>-0.01209250089237101</v>
       </c>
       <c r="I87" t="n">
         <v>5</v>
@@ -4132,25 +4132,25 @@
         <v>45922</v>
       </c>
       <c r="F88" t="n">
-        <v>0.0365943389023488</v>
+        <v>0.03638066369421666</v>
       </c>
       <c r="G88" t="n">
-        <v>0.0282698135608643</v>
+        <v>0.02821265372859229</v>
       </c>
       <c r="H88" t="n">
-        <v>-0.0083245253414845</v>
+        <v>-0.008168009965624373</v>
       </c>
       <c r="I88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K88" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L88" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89">
@@ -4174,13 +4174,13 @@
         <v>45917</v>
       </c>
       <c r="F89" t="n">
-        <v>0.04455179573514183</v>
+        <v>0.04455179573514182</v>
       </c>
       <c r="G89" t="n">
         <v>0.0285092328958587</v>
       </c>
       <c r="H89" t="n">
-        <v>-0.01604256283928314</v>
+        <v>-0.01604256283928312</v>
       </c>
       <c r="I89" t="n">
         <v>5</v>
@@ -4216,10 +4216,10 @@
         <v>45917</v>
       </c>
       <c r="F90" t="n">
-        <v>0.04513845678947007</v>
+        <v>0.04513845678947005</v>
       </c>
       <c r="G90" t="n">
-        <v>0.03226406513218881</v>
+        <v>0.03226406513218879</v>
       </c>
       <c r="H90" t="n">
         <v>-0.01287439165728126</v>
@@ -4258,25 +4258,25 @@
         <v>45922</v>
       </c>
       <c r="F91" t="n">
-        <v>0.0768978041612618</v>
+        <v>0.07483912111116095</v>
       </c>
       <c r="G91" t="n">
-        <v>0.04668152721135205</v>
+        <v>0.04653661344572169</v>
       </c>
       <c r="H91" t="n">
-        <v>-0.03021627694990975</v>
+        <v>-0.02830250766543926</v>
       </c>
       <c r="I91" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J91" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K91" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L91" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92">
@@ -4300,13 +4300,13 @@
         <v>45917</v>
       </c>
       <c r="F92" t="n">
-        <v>0.08153752309307361</v>
+        <v>0.08153752309307355</v>
       </c>
       <c r="G92" t="n">
-        <v>0.05784284381157328</v>
+        <v>0.05784284381157323</v>
       </c>
       <c r="H92" t="n">
-        <v>-0.02369467928150033</v>
+        <v>-0.02369467928150032</v>
       </c>
       <c r="I92" t="n">
         <v>5</v>
@@ -4342,13 +4342,13 @@
         <v>45917</v>
       </c>
       <c r="F93" t="n">
-        <v>0.03304901060746493</v>
+        <v>0.03304901060746495</v>
       </c>
       <c r="G93" t="n">
-        <v>0.027397027323966</v>
+        <v>0.02739702732396601</v>
       </c>
       <c r="H93" t="n">
-        <v>-0.005651983283498932</v>
+        <v>-0.005651983283498935</v>
       </c>
       <c r="I93" t="n">
         <v>5</v>
@@ -4384,13 +4384,13 @@
         <v>45917</v>
       </c>
       <c r="F94" t="n">
-        <v>0.07544077764521201</v>
+        <v>0.07544077764521211</v>
       </c>
       <c r="G94" t="n">
-        <v>0.05455504807487625</v>
+        <v>0.05495773016813484</v>
       </c>
       <c r="H94" t="n">
-        <v>-0.02088572957033576</v>
+        <v>-0.02048304747707727</v>
       </c>
       <c r="I94" t="n">
         <v>5</v>
@@ -4402,7 +4402,7 @@
         <v>18</v>
       </c>
       <c r="L94" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95">
@@ -4426,13 +4426,13 @@
         <v>45917</v>
       </c>
       <c r="F95" t="n">
-        <v>0.05062655711289656</v>
+        <v>0.05062655711289651</v>
       </c>
       <c r="G95" t="n">
-        <v>0.05187962891395864</v>
+        <v>0.05187962891395855</v>
       </c>
       <c r="H95" t="n">
-        <v>0.001253071801062072</v>
+        <v>0.001253071801062045</v>
       </c>
       <c r="I95" t="n">
         <v>5</v>
@@ -4468,13 +4468,13 @@
         <v>45917</v>
       </c>
       <c r="F96" t="n">
-        <v>0.0476729958299417</v>
+        <v>0.04767299582994169</v>
       </c>
       <c r="G96" t="n">
-        <v>0.03903595306049123</v>
+        <v>0.03903595306049121</v>
       </c>
       <c r="H96" t="n">
-        <v>-0.008637042769450473</v>
+        <v>-0.00863704276945048</v>
       </c>
       <c r="I96" t="n">
         <v>5</v>
@@ -4510,13 +4510,13 @@
         <v>45917</v>
       </c>
       <c r="F97" t="n">
-        <v>0.04024805953798257</v>
+        <v>0.04024805953798266</v>
       </c>
       <c r="G97" t="n">
-        <v>0.02587180478941028</v>
+        <v>0.02571894717112846</v>
       </c>
       <c r="H97" t="n">
-        <v>-0.01437625474857229</v>
+        <v>-0.0145291123668542</v>
       </c>
       <c r="I97" t="n">
         <v>5</v>
@@ -4528,7 +4528,7 @@
         <v>25</v>
       </c>
       <c r="L97" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98">
@@ -4555,10 +4555,10 @@
         <v>0.05858731204320907</v>
       </c>
       <c r="G98" t="n">
-        <v>0.0407621928315472</v>
+        <v>0.04105109243415699</v>
       </c>
       <c r="H98" t="n">
-        <v>-0.01782511921166187</v>
+        <v>-0.01753621960905209</v>
       </c>
       <c r="I98" t="n">
         <v>5</v>
@@ -4570,7 +4570,7 @@
         <v>12</v>
       </c>
       <c r="L98" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99">
@@ -4597,10 +4597,10 @@
         <v>0.04255057992829901</v>
       </c>
       <c r="G99" t="n">
-        <v>0.03045503976601936</v>
+        <v>0.0304550397660194</v>
       </c>
       <c r="H99" t="n">
-        <v>-0.01209554016227965</v>
+        <v>-0.01209554016227961</v>
       </c>
       <c r="I99" t="n">
         <v>5</v>
@@ -4636,13 +4636,13 @@
         <v>45917</v>
       </c>
       <c r="F100" t="n">
-        <v>0.02970656858327371</v>
+        <v>0.0297065685832737</v>
       </c>
       <c r="G100" t="n">
-        <v>0.02337043210005382</v>
+        <v>0.02337043210005384</v>
       </c>
       <c r="H100" t="n">
-        <v>-0.006336136483219887</v>
+        <v>-0.006336136483219863</v>
       </c>
       <c r="I100" t="n">
         <v>5</v>
@@ -4678,13 +4678,13 @@
         <v>45917</v>
       </c>
       <c r="F101" t="n">
-        <v>0.03331212379673355</v>
+        <v>0.03331212379673363</v>
       </c>
       <c r="G101" t="n">
-        <v>0.02808285490147273</v>
+        <v>0.02827171495175317</v>
       </c>
       <c r="H101" t="n">
-        <v>-0.005229268895260823</v>
+        <v>-0.00504040884498046</v>
       </c>
       <c r="I101" t="n">
         <v>5</v>
@@ -4696,7 +4696,7 @@
         <v>18</v>
       </c>
       <c r="L101" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="102">
@@ -4723,10 +4723,10 @@
         <v>0.02817059210404283</v>
       </c>
       <c r="G102" t="n">
-        <v>0.0172291240582471</v>
+        <v>0.01722912405824712</v>
       </c>
       <c r="H102" t="n">
-        <v>-0.01094146804579572</v>
+        <v>-0.01094146804579571</v>
       </c>
       <c r="I102" t="n">
         <v>5</v>
@@ -4762,10 +4762,10 @@
         <v>45917</v>
       </c>
       <c r="F103" t="n">
-        <v>0.01951955672491874</v>
+        <v>0.01951955672491875</v>
       </c>
       <c r="G103" t="n">
-        <v>0.01487138815921951</v>
+        <v>0.01487138815921952</v>
       </c>
       <c r="H103" t="n">
         <v>-0.00464816856569923</v>
@@ -4804,13 +4804,13 @@
         <v>45917</v>
       </c>
       <c r="F104" t="n">
-        <v>0.05937944413325686</v>
+        <v>0.05937944413325685</v>
       </c>
       <c r="G104" t="n">
-        <v>0.04053320969706162</v>
+        <v>0.04089089230165448</v>
       </c>
       <c r="H104" t="n">
-        <v>-0.01884623443619524</v>
+        <v>-0.01848855183160237</v>
       </c>
       <c r="I104" t="n">
         <v>5</v>
@@ -4822,7 +4822,7 @@
         <v>13</v>
       </c>
       <c r="L104" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105">
@@ -4846,13 +4846,13 @@
         <v>45917</v>
       </c>
       <c r="F105" t="n">
-        <v>0.0491471752268131</v>
+        <v>0.04914717522681311</v>
       </c>
       <c r="G105" t="n">
-        <v>0.03216618788592523</v>
+        <v>0.03216618788592524</v>
       </c>
       <c r="H105" t="n">
-        <v>-0.01698098734088788</v>
+        <v>-0.01698098734088787</v>
       </c>
       <c r="I105" t="n">
         <v>5</v>
@@ -4888,13 +4888,13 @@
         <v>45917</v>
       </c>
       <c r="F106" t="n">
-        <v>0.03873989892762818</v>
+        <v>0.03873989892762816</v>
       </c>
       <c r="G106" t="n">
-        <v>0.02473627701501018</v>
+        <v>0.02473627701501019</v>
       </c>
       <c r="H106" t="n">
-        <v>-0.014003621912618</v>
+        <v>-0.01400362191261797</v>
       </c>
       <c r="I106" t="n">
         <v>5</v>
@@ -4972,13 +4972,13 @@
         <v>45917</v>
       </c>
       <c r="F108" t="n">
-        <v>0.03758224182248273</v>
+        <v>0.03758224182248276</v>
       </c>
       <c r="G108" t="n">
-        <v>0.02084772041673932</v>
+        <v>0.02077786062155969</v>
       </c>
       <c r="H108" t="n">
-        <v>-0.01673452140574341</v>
+        <v>-0.01680438120092307</v>
       </c>
       <c r="I108" t="n">
         <v>5</v>
@@ -4990,7 +4990,7 @@
         <v>17</v>
       </c>
       <c r="L108" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109">
@@ -5014,10 +5014,10 @@
         <v>45917</v>
       </c>
       <c r="F109" t="n">
-        <v>0.04089730154050022</v>
+        <v>0.04089730154050027</v>
       </c>
       <c r="G109" t="n">
-        <v>0.0307301328905502</v>
+        <v>0.03073013289055024</v>
       </c>
       <c r="H109" t="n">
         <v>-0.01016716864995003</v>
@@ -5059,10 +5059,10 @@
         <v>0.04024092776073378</v>
       </c>
       <c r="G110" t="n">
-        <v>0.02655978245469491</v>
+        <v>0.02649828933901129</v>
       </c>
       <c r="H110" t="n">
-        <v>-0.01368114530603887</v>
+        <v>-0.01374263842172248</v>
       </c>
       <c r="I110" t="n">
         <v>5</v>
@@ -5074,7 +5074,7 @@
         <v>22</v>
       </c>
       <c r="L110" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="111">
@@ -5098,13 +5098,13 @@
         <v>45917</v>
       </c>
       <c r="F111" t="n">
-        <v>0.04974003331171842</v>
+        <v>0.0497400333117184</v>
       </c>
       <c r="G111" t="n">
-        <v>0.03533797655294108</v>
+        <v>0.03533797655294105</v>
       </c>
       <c r="H111" t="n">
-        <v>-0.01440205675877734</v>
+        <v>-0.01440205675877735</v>
       </c>
       <c r="I111" t="n">
         <v>5</v>
@@ -5227,10 +5227,10 @@
         <v>0.004391502518619216</v>
       </c>
       <c r="G114" t="n">
-        <v>0.004379167552573275</v>
+        <v>0.004379167552573276</v>
       </c>
       <c r="H114" t="n">
-        <v>-1.233496604594129e-05</v>
+        <v>-1.233496604594042e-05</v>
       </c>
       <c r="I114" t="n">
         <v>5</v>
@@ -5434,25 +5434,25 @@
         <v>45922</v>
       </c>
       <c r="F119" t="n">
-        <v>0.008197202271980472</v>
+        <v>0.009718509492492198</v>
       </c>
       <c r="G119" t="n">
-        <v>0.004603874928064454</v>
+        <v>0.004146848526284551</v>
       </c>
       <c r="H119" t="n">
-        <v>-0.003593327343916018</v>
+        <v>-0.005571660966207647</v>
       </c>
       <c r="I119" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J119" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K119" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L119" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="120">
@@ -5479,10 +5479,10 @@
         <v>0.01075246610797691</v>
       </c>
       <c r="G120" t="n">
-        <v>0.006287655223325719</v>
+        <v>0.007034959589718373</v>
       </c>
       <c r="H120" t="n">
-        <v>-0.004464810884651194</v>
+        <v>-0.003717506518258539</v>
       </c>
       <c r="I120" t="n">
         <v>5</v>
@@ -5518,25 +5518,25 @@
         <v>45922</v>
       </c>
       <c r="F121" t="n">
-        <v>0.007097145472068337</v>
+        <v>0.009992959253121384</v>
       </c>
       <c r="G121" t="n">
-        <v>0.00383865034451975</v>
+        <v>0.003654430626184111</v>
       </c>
       <c r="H121" t="n">
-        <v>-0.003258495127548586</v>
+        <v>-0.006338528626937272</v>
       </c>
       <c r="I121" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J121" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K121" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L121" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="122">
@@ -5644,25 +5644,25 @@
         <v>45922</v>
       </c>
       <c r="F124" t="n">
-        <v>0.003042594951964464</v>
+        <v>0.005258749556864466</v>
       </c>
       <c r="G124" t="n">
-        <v>0.002962962962962963</v>
+        <v>0.003839633447880871</v>
       </c>
       <c r="H124" t="n">
-        <v>-7.963198900150107e-05</v>
+        <v>-0.001419116108983595</v>
       </c>
       <c r="I124" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J124" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K124" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L124" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125">
@@ -5899,10 +5899,10 @@
         <v>0.0069740508084855</v>
       </c>
       <c r="G130" t="n">
-        <v>0.005830747514244294</v>
+        <v>0.005787479718961531</v>
       </c>
       <c r="H130" t="n">
-        <v>-0.001143303294241206</v>
+        <v>-0.001186571089523969</v>
       </c>
       <c r="I130" t="n">
         <v>5</v>
@@ -5914,7 +5914,7 @@
         <v>30</v>
       </c>
       <c r="L130" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="131">
@@ -5983,10 +5983,10 @@
         <v>0.007956456322392478</v>
       </c>
       <c r="G132" t="n">
-        <v>0.006765006702328969</v>
+        <v>0.00702013984388743</v>
       </c>
       <c r="H132" t="n">
-        <v>-0.001191449620063509</v>
+        <v>-0.0009363164785050476</v>
       </c>
       <c r="I132" t="n">
         <v>5</v>
@@ -5998,7 +5998,7 @@
         <v>19</v>
       </c>
       <c r="L132" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="133">
@@ -6067,10 +6067,10 @@
         <v>0.0123733435284104</v>
       </c>
       <c r="G134" t="n">
-        <v>0.01228751145293127</v>
+        <v>0.01191016698712307</v>
       </c>
       <c r="H134" t="n">
-        <v>-8.583207547912738e-05</v>
+        <v>-0.0004631765412873318</v>
       </c>
       <c r="I134" t="n">
         <v>5</v>
@@ -6082,7 +6082,7 @@
         <v>18</v>
       </c>
       <c r="L134" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="135">
@@ -6106,25 +6106,25 @@
         <v>45922</v>
       </c>
       <c r="F135" t="n">
-        <v>0.01378419452887538</v>
+        <v>0.01238396580165264</v>
       </c>
       <c r="G135" t="n">
-        <v>0.007425742574257425</v>
+        <v>0.004243281471004243</v>
       </c>
       <c r="H135" t="n">
-        <v>-0.006358451954617953</v>
+        <v>-0.008140684330648396</v>
       </c>
       <c r="I135" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J135" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K135" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L135" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136">
@@ -6274,25 +6274,25 @@
         <v>45922</v>
       </c>
       <c r="F139" t="n">
-        <v>0.01264469876348329</v>
+        <v>0.01454888836498939</v>
       </c>
       <c r="G139" t="n">
-        <v>0.006557947290882305</v>
+        <v>0.01161834167218241</v>
       </c>
       <c r="H139" t="n">
-        <v>-0.006086751472600988</v>
+        <v>-0.002930546692806985</v>
       </c>
       <c r="I139" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J139" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K139" t="n">
+        <v>7</v>
+      </c>
+      <c r="L139" t="n">
         <v>6</v>
-      </c>
-      <c r="L139" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="140">
@@ -6442,25 +6442,25 @@
         <v>45922</v>
       </c>
       <c r="F143" t="n">
-        <v>0.004320466579694575</v>
+        <v>0.004718957049074338</v>
       </c>
       <c r="G143" t="n">
-        <v>0.01146873843877174</v>
+        <v>0.007258249211634339</v>
       </c>
       <c r="H143" t="n">
-        <v>0.00714827185907716</v>
+        <v>0.002539292162560001</v>
       </c>
       <c r="I143" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J143" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K143" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L143" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144">
@@ -6568,25 +6568,25 @@
         <v>45922</v>
       </c>
       <c r="F146" t="n">
-        <v>0.004595053573774184</v>
+        <v>0.008545825189533665</v>
       </c>
       <c r="G146" t="n">
-        <v>0.005705416399058017</v>
+        <v>0.009127119055714771</v>
       </c>
       <c r="H146" t="n">
-        <v>0.001110362825283834</v>
+        <v>0.0005812938661811061</v>
       </c>
       <c r="I146" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J146" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K146" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L146" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147">
@@ -6697,10 +6697,10 @@
         <v>0.01363628330188187</v>
       </c>
       <c r="G149" t="n">
-        <v>0.007753173043378654</v>
+        <v>0.007912225525256486</v>
       </c>
       <c r="H149" t="n">
-        <v>-0.005883110258503217</v>
+        <v>-0.005724057776625385</v>
       </c>
       <c r="I149" t="n">
         <v>5</v>
@@ -6712,7 +6712,7 @@
         <v>18</v>
       </c>
       <c r="L149" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150">
@@ -6823,10 +6823,10 @@
         <v>0.00683847560605484</v>
       </c>
       <c r="G152" t="n">
-        <v>0.009745552873552946</v>
+        <v>0.009502373397282559</v>
       </c>
       <c r="H152" t="n">
-        <v>0.002907077267498106</v>
+        <v>0.002663897791227719</v>
       </c>
       <c r="I152" t="n">
         <v>5</v>
@@ -6838,7 +6838,7 @@
         <v>25</v>
       </c>
       <c r="L152" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="153">
@@ -6865,10 +6865,10 @@
         <v>0.01410824361901666</v>
       </c>
       <c r="G153" t="n">
-        <v>0.008008682716253917</v>
+        <v>0.008388048842356289</v>
       </c>
       <c r="H153" t="n">
-        <v>-0.006099560902762745</v>
+        <v>-0.005720194776660373</v>
       </c>
       <c r="I153" t="n">
         <v>5</v>
@@ -6880,7 +6880,7 @@
         <v>12</v>
       </c>
       <c r="L153" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154">
@@ -6907,10 +6907,10 @@
         <v>0.005931388412928523</v>
       </c>
       <c r="G154" t="n">
-        <v>0.00560127553151649</v>
+        <v>0.006030214622165618</v>
       </c>
       <c r="H154" t="n">
-        <v>-0.0003301128814120332</v>
+        <v>9.882620923709444e-05</v>
       </c>
       <c r="I154" t="n">
         <v>5</v>
@@ -6991,10 +6991,10 @@
         <v>0.005299482805768059</v>
       </c>
       <c r="G156" t="n">
-        <v>0.007412547120926246</v>
+        <v>0.007417941266065938</v>
       </c>
       <c r="H156" t="n">
-        <v>0.002113064315158186</v>
+        <v>0.002118458460297879</v>
       </c>
       <c r="I156" t="n">
         <v>5</v>
@@ -7006,7 +7006,7 @@
         <v>18</v>
       </c>
       <c r="L156" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="157">
@@ -7117,10 +7117,10 @@
         <v>0.01195177480421316</v>
       </c>
       <c r="G159" t="n">
-        <v>0.01483795765833191</v>
+        <v>0.01479466781649737</v>
       </c>
       <c r="H159" t="n">
-        <v>0.002886182854118747</v>
+        <v>0.002842893012284209</v>
       </c>
       <c r="I159" t="n">
         <v>5</v>
@@ -7132,7 +7132,7 @@
         <v>13</v>
       </c>
       <c r="L159" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160">
@@ -7285,10 +7285,10 @@
         <v>0.01016623815325596</v>
       </c>
       <c r="G163" t="n">
-        <v>0.00581168943258708</v>
+        <v>0.005923916006059515</v>
       </c>
       <c r="H163" t="n">
-        <v>-0.004354548720668878</v>
+        <v>-0.004242322147196442</v>
       </c>
       <c r="I163" t="n">
         <v>5</v>
@@ -7300,7 +7300,7 @@
         <v>17</v>
       </c>
       <c r="L163" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="164">
@@ -7369,10 +7369,10 @@
         <v>0.008225933412392215</v>
       </c>
       <c r="G165" t="n">
-        <v>0.004186070808862074</v>
+        <v>0.004018627976507591</v>
       </c>
       <c r="H165" t="n">
-        <v>-0.004039862603530142</v>
+        <v>-0.004207305435884624</v>
       </c>
       <c r="I165" t="n">
         <v>5</v>
@@ -7384,7 +7384,7 @@
         <v>22</v>
       </c>
       <c r="L165" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="166">
@@ -7450,13 +7450,13 @@
         <v>45917</v>
       </c>
       <c r="F167" t="n">
-        <v>0.6464537154814753</v>
+        <v>0.6907806382077675</v>
       </c>
       <c r="G167" t="n">
-        <v>0.371908190855431</v>
+        <v>0.4521376859529998</v>
       </c>
       <c r="H167" t="n">
-        <v>-0.2745455246260444</v>
+        <v>-0.2386429522547677</v>
       </c>
       <c r="I167" t="n">
         <v>5</v>
@@ -7492,13 +7492,13 @@
         <v>45917</v>
       </c>
       <c r="F168" t="n">
-        <v>0.6530246180497322</v>
+        <v>0.7130854901508369</v>
       </c>
       <c r="G168" t="n">
-        <v>0.4263342417210072</v>
+        <v>0.526725749419831</v>
       </c>
       <c r="H168" t="n">
-        <v>-0.226690376328725</v>
+        <v>-0.1863597407310059</v>
       </c>
       <c r="I168" t="n">
         <v>5</v>
@@ -7534,13 +7534,13 @@
         <v>45917</v>
       </c>
       <c r="F169" t="n">
-        <v>0.5416896258450016</v>
+        <v>0.5746189948114916</v>
       </c>
       <c r="G169" t="n">
-        <v>0.3709011523214762</v>
+        <v>0.4170527736652895</v>
       </c>
       <c r="H169" t="n">
-        <v>-0.1707884735235253</v>
+        <v>-0.1575662211462021</v>
       </c>
       <c r="I169" t="n">
         <v>5</v>
@@ -7576,13 +7576,13 @@
         <v>45917</v>
       </c>
       <c r="F170" t="n">
-        <v>0.6160440562023353</v>
+        <v>0.6655156904766418</v>
       </c>
       <c r="G170" t="n">
-        <v>0.3005461077199161</v>
+        <v>0.3941441987354659</v>
       </c>
       <c r="H170" t="n">
-        <v>-0.3154979484824192</v>
+        <v>-0.2713714917411759</v>
       </c>
       <c r="I170" t="n">
         <v>5</v>
@@ -7618,13 +7618,13 @@
         <v>45917</v>
       </c>
       <c r="F171" t="n">
-        <v>0.6453704047840737</v>
+        <v>0.6800942005688255</v>
       </c>
       <c r="G171" t="n">
-        <v>0.4048154725212611</v>
+        <v>0.4647075761350102</v>
       </c>
       <c r="H171" t="n">
-        <v>-0.2405549322628126</v>
+        <v>-0.2153866244338153</v>
       </c>
       <c r="I171" t="n">
         <v>5</v>
@@ -7660,13 +7660,13 @@
         <v>45917</v>
       </c>
       <c r="F172" t="n">
-        <v>0.5804033589664498</v>
+        <v>0.6107735024327853</v>
       </c>
       <c r="G172" t="n">
-        <v>0.3709097647469159</v>
+        <v>0.417993265697872</v>
       </c>
       <c r="H172" t="n">
-        <v>-0.2094935942195339</v>
+        <v>-0.1927802367349132</v>
       </c>
       <c r="I172" t="n">
         <v>5</v>
@@ -7702,13 +7702,13 @@
         <v>45917</v>
       </c>
       <c r="F173" t="n">
-        <v>0.6217725557226857</v>
+        <v>0.6638956784559255</v>
       </c>
       <c r="G173" t="n">
-        <v>0.4049528492863623</v>
+        <v>0.4733762685508001</v>
       </c>
       <c r="H173" t="n">
-        <v>-0.2168197064363234</v>
+        <v>-0.1905194099051254</v>
       </c>
       <c r="I173" t="n">
         <v>5</v>
@@ -7744,25 +7744,25 @@
         <v>45922</v>
       </c>
       <c r="F174" t="n">
-        <v>0.7161972492137257</v>
+        <v>0.7402567564348365</v>
       </c>
       <c r="G174" t="n">
-        <v>0.290812963499598</v>
+        <v>0.3513115031256053</v>
       </c>
       <c r="H174" t="n">
-        <v>-0.4253842857141278</v>
+        <v>-0.3889452533092311</v>
       </c>
       <c r="I174" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J174" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K174" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L174" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="175">
@@ -7786,13 +7786,13 @@
         <v>45917</v>
       </c>
       <c r="F175" t="n">
-        <v>0.6145445034843791</v>
+        <v>0.6620862111225867</v>
       </c>
       <c r="G175" t="n">
-        <v>0.3900191398936098</v>
+        <v>0.4682361158467061</v>
       </c>
       <c r="H175" t="n">
-        <v>-0.2245253635907692</v>
+        <v>-0.1938500952758806</v>
       </c>
       <c r="I175" t="n">
         <v>5</v>
@@ -7828,25 +7828,25 @@
         <v>45922</v>
       </c>
       <c r="F176" t="n">
-        <v>0.6875728638089361</v>
+        <v>0.7191509447232064</v>
       </c>
       <c r="G176" t="n">
-        <v>0.2713811317076174</v>
+        <v>0.3564600492241725</v>
       </c>
       <c r="H176" t="n">
-        <v>-0.4161917321013187</v>
+        <v>-0.3626908954990339</v>
       </c>
       <c r="I176" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J176" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K176" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L176" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="177">
@@ -7870,13 +7870,13 @@
         <v>45917</v>
       </c>
       <c r="F177" t="n">
-        <v>0.6178619383567003</v>
+        <v>0.6620423131894438</v>
       </c>
       <c r="G177" t="n">
-        <v>0.3457349882766957</v>
+        <v>0.4242383078788601</v>
       </c>
       <c r="H177" t="n">
-        <v>-0.2721269500800046</v>
+        <v>-0.2378040053105837</v>
       </c>
       <c r="I177" t="n">
         <v>5</v>
@@ -7912,13 +7912,13 @@
         <v>45917</v>
       </c>
       <c r="F178" t="n">
-        <v>0.5789480201059455</v>
+        <v>0.6263186969818848</v>
       </c>
       <c r="G178" t="n">
-        <v>0.3570442470494058</v>
+        <v>0.4314217322143571</v>
       </c>
       <c r="H178" t="n">
-        <v>-0.2219037730565396</v>
+        <v>-0.1948969647675277</v>
       </c>
       <c r="I178" t="n">
         <v>5</v>
@@ -7954,25 +7954,25 @@
         <v>45922</v>
       </c>
       <c r="F179" t="n">
-        <v>0.7037057952549843</v>
+        <v>0.7161907399619436</v>
       </c>
       <c r="G179" t="n">
-        <v>0.3229415954415955</v>
+        <v>0.3503480923429377</v>
       </c>
       <c r="H179" t="n">
-        <v>-0.3807641998133889</v>
+        <v>-0.3658426476190059</v>
       </c>
       <c r="I179" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J179" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K179" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L179" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180">
@@ -7996,13 +7996,13 @@
         <v>45917</v>
       </c>
       <c r="F180" t="n">
-        <v>0.6087294649936781</v>
+        <v>0.6399617357287986</v>
       </c>
       <c r="G180" t="n">
-        <v>0.4450321706526002</v>
+        <v>0.4900888326343636</v>
       </c>
       <c r="H180" t="n">
-        <v>-0.1636972943410779</v>
+        <v>-0.1498729030944349</v>
       </c>
       <c r="I180" t="n">
         <v>5</v>
@@ -8038,13 +8038,13 @@
         <v>45917</v>
       </c>
       <c r="F181" t="n">
-        <v>0.5735481939010427</v>
+        <v>0.6069217499342953</v>
       </c>
       <c r="G181" t="n">
-        <v>0.3843989274627145</v>
+        <v>0.4339600254828112</v>
       </c>
       <c r="H181" t="n">
-        <v>-0.1891492664383282</v>
+        <v>-0.1729617244514841</v>
       </c>
       <c r="I181" t="n">
         <v>5</v>
@@ -8080,13 +8080,13 @@
         <v>45917</v>
       </c>
       <c r="F182" t="n">
-        <v>0.5375285660196725</v>
+        <v>0.5867288654764286</v>
       </c>
       <c r="G182" t="n">
-        <v>0.307211437237277</v>
+        <v>0.3822018792130765</v>
       </c>
       <c r="H182" t="n">
-        <v>-0.2303171287823955</v>
+        <v>-0.2045269862633521</v>
       </c>
       <c r="I182" t="n">
         <v>5</v>
@@ -8122,13 +8122,13 @@
         <v>45917</v>
       </c>
       <c r="F183" t="n">
-        <v>0.5498741958602317</v>
+        <v>0.5825007992754728</v>
       </c>
       <c r="G183" t="n">
-        <v>0.3502181400975065</v>
+        <v>0.3975476572539788</v>
       </c>
       <c r="H183" t="n">
-        <v>-0.1996560557627252</v>
+        <v>-0.184953142021494</v>
       </c>
       <c r="I183" t="n">
         <v>5</v>
@@ -8164,13 +8164,13 @@
         <v>45917</v>
       </c>
       <c r="F184" t="n">
-        <v>0.5807448389353379</v>
+        <v>0.615951292221531</v>
       </c>
       <c r="G184" t="n">
-        <v>0.3708933355544773</v>
+        <v>0.4248524491773938</v>
       </c>
       <c r="H184" t="n">
-        <v>-0.2098515033808606</v>
+        <v>-0.1910988430441372</v>
       </c>
       <c r="I184" t="n">
         <v>5</v>
@@ -8206,13 +8206,13 @@
         <v>45917</v>
       </c>
       <c r="F185" t="n">
-        <v>0.5625559225374808</v>
+        <v>0.6124519425543774</v>
       </c>
       <c r="G185" t="n">
-        <v>0.3534363491797999</v>
+        <v>0.4341514020992709</v>
       </c>
       <c r="H185" t="n">
-        <v>-0.2091195733576808</v>
+        <v>-0.1783005404551065</v>
       </c>
       <c r="I185" t="n">
         <v>5</v>
@@ -8224,7 +8224,7 @@
         <v>30</v>
       </c>
       <c r="L185" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="186">
@@ -8248,13 +8248,13 @@
         <v>45917</v>
       </c>
       <c r="F186" t="n">
-        <v>0.6098658738748753</v>
+        <v>0.6501337723049949</v>
       </c>
       <c r="G186" t="n">
-        <v>0.4002846403550165</v>
+        <v>0.4641248447858652</v>
       </c>
       <c r="H186" t="n">
-        <v>-0.2095812335198589</v>
+        <v>-0.1860089275191297</v>
       </c>
       <c r="I186" t="n">
         <v>5</v>
@@ -8290,13 +8290,13 @@
         <v>45917</v>
       </c>
       <c r="F187" t="n">
-        <v>0.5669496671282444</v>
+        <v>0.6097400819738603</v>
       </c>
       <c r="G187" t="n">
-        <v>0.4014177937140449</v>
+        <v>0.4700622179102185</v>
       </c>
       <c r="H187" t="n">
-        <v>-0.1655318734141994</v>
+        <v>-0.1396778640636418</v>
       </c>
       <c r="I187" t="n">
         <v>5</v>
@@ -8308,7 +8308,7 @@
         <v>19</v>
       </c>
       <c r="L187" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="188">
@@ -8332,13 +8332,13 @@
         <v>45917</v>
       </c>
       <c r="F188" t="n">
-        <v>0.6588823329660288</v>
+        <v>0.7036541096980025</v>
       </c>
       <c r="G188" t="n">
-        <v>0.3925256937531532</v>
+        <v>0.474665778589431</v>
       </c>
       <c r="H188" t="n">
-        <v>-0.2663566392128757</v>
+        <v>-0.2289883311085714</v>
       </c>
       <c r="I188" t="n">
         <v>5</v>
@@ -8374,13 +8374,13 @@
         <v>45917</v>
       </c>
       <c r="F189" t="n">
-        <v>0.6576678196587432</v>
+        <v>0.6932417068746184</v>
       </c>
       <c r="G189" t="n">
-        <v>0.4840793739841214</v>
+        <v>0.5441643016641815</v>
       </c>
       <c r="H189" t="n">
-        <v>-0.1735884456746218</v>
+        <v>-0.1490774052104369</v>
       </c>
       <c r="I189" t="n">
         <v>5</v>
@@ -8392,7 +8392,7 @@
         <v>18</v>
       </c>
       <c r="L189" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="190">
@@ -8416,25 +8416,25 @@
         <v>45922</v>
       </c>
       <c r="F190" t="n">
-        <v>0.6564589665653495</v>
+        <v>0.699937448450459</v>
       </c>
       <c r="G190" t="n">
-        <v>0.2967518690644574</v>
+        <v>0.3899040804440588</v>
       </c>
       <c r="H190" t="n">
-        <v>-0.3597070975008921</v>
+        <v>-0.3100333680064002</v>
       </c>
       <c r="I190" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J190" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K190" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L190" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="191">
@@ -8458,13 +8458,13 @@
         <v>45917</v>
       </c>
       <c r="F191" t="n">
-        <v>0.6309909584914334</v>
+        <v>0.6820976845807165</v>
       </c>
       <c r="G191" t="n">
-        <v>0.4397771865341064</v>
+        <v>0.5191866108761373</v>
       </c>
       <c r="H191" t="n">
-        <v>-0.191213771957327</v>
+        <v>-0.1629110737045792</v>
       </c>
       <c r="I191" t="n">
         <v>5</v>
@@ -8500,13 +8500,13 @@
         <v>45917</v>
       </c>
       <c r="F192" t="n">
-        <v>0.558820066541205</v>
+        <v>0.6127894954943909</v>
       </c>
       <c r="G192" t="n">
-        <v>0.3651250591473283</v>
+        <v>0.4446830834524121</v>
       </c>
       <c r="H192" t="n">
-        <v>-0.1936950073938766</v>
+        <v>-0.1681064120419787</v>
       </c>
       <c r="I192" t="n">
         <v>5</v>
@@ -8542,13 +8542,13 @@
         <v>45917</v>
       </c>
       <c r="F193" t="n">
-        <v>0.6604979262092759</v>
+        <v>0.714225131361909</v>
       </c>
       <c r="G193" t="n">
-        <v>0.4064769484404944</v>
+        <v>0.5027598569769242</v>
       </c>
       <c r="H193" t="n">
-        <v>-0.2540209777687815</v>
+        <v>-0.2114652743849849</v>
       </c>
       <c r="I193" t="n">
         <v>5</v>
@@ -8584,25 +8584,25 @@
         <v>45922</v>
       </c>
       <c r="F194" t="n">
-        <v>0.6901144435674822</v>
+        <v>0.7222930483092282</v>
       </c>
       <c r="G194" t="n">
-        <v>0.3573211654935342</v>
+        <v>0.423068977188167</v>
       </c>
       <c r="H194" t="n">
-        <v>-0.332793278073948</v>
+        <v>-0.2992240711210613</v>
       </c>
       <c r="I194" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J194" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K194" t="n">
+        <v>7</v>
+      </c>
+      <c r="L194" t="n">
         <v>6</v>
-      </c>
-      <c r="L194" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="195">
@@ -8626,13 +8626,13 @@
         <v>45917</v>
       </c>
       <c r="F195" t="n">
-        <v>0.6010085002308752</v>
+        <v>0.6630392275380903</v>
       </c>
       <c r="G195" t="n">
-        <v>0.3534262485481998</v>
+        <v>0.456148105131845</v>
       </c>
       <c r="H195" t="n">
-        <v>-0.2475822516826753</v>
+        <v>-0.2068911224062453</v>
       </c>
       <c r="I195" t="n">
         <v>5</v>
@@ -8668,13 +8668,13 @@
         <v>45917</v>
       </c>
       <c r="F196" t="n">
-        <v>0.6953558512799348</v>
+        <v>0.715010312487681</v>
       </c>
       <c r="G196" t="n">
-        <v>0.5191752866344771</v>
+        <v>0.5508614636591314</v>
       </c>
       <c r="H196" t="n">
-        <v>-0.1761805646454577</v>
+        <v>-0.1641488488285496</v>
       </c>
       <c r="I196" t="n">
         <v>5</v>
@@ -8710,13 +8710,13 @@
         <v>45917</v>
       </c>
       <c r="F197" t="n">
-        <v>0.6252190107372128</v>
+        <v>0.6636141101814665</v>
       </c>
       <c r="G197" t="n">
-        <v>0.4017798298385312</v>
+        <v>0.4647285937056595</v>
       </c>
       <c r="H197" t="n">
-        <v>-0.2234391808986815</v>
+        <v>-0.198885516475807</v>
       </c>
       <c r="I197" t="n">
         <v>5</v>
@@ -8752,25 +8752,25 @@
         <v>45922</v>
       </c>
       <c r="F198" t="n">
-        <v>0.6136597344793185</v>
+        <v>0.6376587442404166</v>
       </c>
       <c r="G198" t="n">
-        <v>0.2339622641509434</v>
+        <v>0.2717973765086169</v>
       </c>
       <c r="H198" t="n">
-        <v>-0.3796974703283751</v>
+        <v>-0.3658613677317997</v>
       </c>
       <c r="I198" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J198" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K198" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L198" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="199">
@@ -8794,13 +8794,13 @@
         <v>45917</v>
       </c>
       <c r="F199" t="n">
-        <v>0.5874836192517017</v>
+        <v>0.618986189364061</v>
       </c>
       <c r="G199" t="n">
-        <v>0.3563834082955553</v>
+        <v>0.4076225569044022</v>
       </c>
       <c r="H199" t="n">
-        <v>-0.2311002109561464</v>
+        <v>-0.2113636324596588</v>
       </c>
       <c r="I199" t="n">
         <v>5</v>
@@ -8836,13 +8836,13 @@
         <v>45917</v>
       </c>
       <c r="F200" t="n">
-        <v>0.6784072113051776</v>
+        <v>0.7015551483898397</v>
       </c>
       <c r="G200" t="n">
-        <v>0.4964533462964875</v>
+        <v>0.5335522915903963</v>
       </c>
       <c r="H200" t="n">
-        <v>-0.18195386500869</v>
+        <v>-0.1680028567994434</v>
       </c>
       <c r="I200" t="n">
         <v>5</v>
@@ -8878,25 +8878,25 @@
         <v>45922</v>
       </c>
       <c r="F201" t="n">
-        <v>0.6045063894466233</v>
+        <v>0.6406636871635282</v>
       </c>
       <c r="G201" t="n">
-        <v>0.2868229501177478</v>
+        <v>0.3612204033829332</v>
       </c>
       <c r="H201" t="n">
-        <v>-0.3176834393288755</v>
+        <v>-0.279443283780595</v>
       </c>
       <c r="I201" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J201" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K201" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L201" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="202">
@@ -8920,13 +8920,13 @@
         <v>45917</v>
       </c>
       <c r="F202" t="n">
-        <v>0.5785815838309719</v>
+        <v>0.6241169020306501</v>
       </c>
       <c r="G202" t="n">
-        <v>0.3894126994810129</v>
+        <v>0.4575393727284964</v>
       </c>
       <c r="H202" t="n">
-        <v>-0.189168884349959</v>
+        <v>-0.1665775293021536</v>
       </c>
       <c r="I202" t="n">
         <v>5</v>
@@ -8962,13 +8962,13 @@
         <v>45917</v>
       </c>
       <c r="F203" t="n">
-        <v>0.5960018660614204</v>
+        <v>0.6427415597977841</v>
       </c>
       <c r="G203" t="n">
-        <v>0.3642854842313104</v>
+        <v>0.439703700132166</v>
       </c>
       <c r="H203" t="n">
-        <v>-0.23171638183011</v>
+        <v>-0.2030378596656181</v>
       </c>
       <c r="I203" t="n">
         <v>5</v>
@@ -9004,13 +9004,13 @@
         <v>45917</v>
       </c>
       <c r="F204" t="n">
-        <v>0.6557358872448966</v>
+        <v>0.6770443993757664</v>
       </c>
       <c r="G204" t="n">
-        <v>0.4595460868219008</v>
+        <v>0.5000190938507156</v>
       </c>
       <c r="H204" t="n">
-        <v>-0.1961898004229958</v>
+        <v>-0.1770253055250508</v>
       </c>
       <c r="I204" t="n">
         <v>5</v>
@@ -9022,7 +9022,7 @@
         <v>18</v>
       </c>
       <c r="L204" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="205">
@@ -9046,13 +9046,13 @@
         <v>45917</v>
       </c>
       <c r="F205" t="n">
-        <v>0.6248230306110824</v>
+        <v>0.6684876902354063</v>
       </c>
       <c r="G205" t="n">
-        <v>0.394514543443918</v>
+        <v>0.4671270223248231</v>
       </c>
       <c r="H205" t="n">
-        <v>-0.2303084871671644</v>
+        <v>-0.2013606679105833</v>
       </c>
       <c r="I205" t="n">
         <v>5</v>
@@ -9088,13 +9088,13 @@
         <v>45917</v>
       </c>
       <c r="F206" t="n">
-        <v>0.616917086650557</v>
+        <v>0.6294112508864101</v>
       </c>
       <c r="G206" t="n">
-        <v>0.4152684107550061</v>
+        <v>0.4364062911370876</v>
       </c>
       <c r="H206" t="n">
-        <v>-0.2016486758955509</v>
+        <v>-0.1930049597493226</v>
       </c>
       <c r="I206" t="n">
         <v>5</v>
@@ -9130,13 +9130,13 @@
         <v>45917</v>
       </c>
       <c r="F207" t="n">
-        <v>0.6015875867972553</v>
+        <v>0.6406084581176195</v>
       </c>
       <c r="G207" t="n">
-        <v>0.4214376033459102</v>
+        <v>0.4745395208726821</v>
       </c>
       <c r="H207" t="n">
-        <v>-0.1801499834513451</v>
+        <v>-0.1660689372449373</v>
       </c>
       <c r="I207" t="n">
         <v>5</v>
@@ -9148,7 +9148,7 @@
         <v>25</v>
       </c>
       <c r="L207" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="208">
@@ -9172,13 +9172,13 @@
         <v>45917</v>
       </c>
       <c r="F208" t="n">
-        <v>0.598931875986122</v>
+        <v>0.64250699734619</v>
       </c>
       <c r="G208" t="n">
-        <v>0.4290589558030997</v>
+        <v>0.4987925774340809</v>
       </c>
       <c r="H208" t="n">
-        <v>-0.1698729201830222</v>
+        <v>-0.1437144199121091</v>
       </c>
       <c r="I208" t="n">
         <v>5</v>
@@ -9190,7 +9190,7 @@
         <v>12</v>
       </c>
       <c r="L208" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="209">
@@ -9214,13 +9214,13 @@
         <v>45917</v>
       </c>
       <c r="F209" t="n">
-        <v>0.5697293421248919</v>
+        <v>0.6267288620046462</v>
       </c>
       <c r="G209" t="n">
-        <v>0.3828729318483694</v>
+        <v>0.4671526779472688</v>
       </c>
       <c r="H209" t="n">
-        <v>-0.1868564102765225</v>
+        <v>-0.1595761840573773</v>
       </c>
       <c r="I209" t="n">
         <v>5</v>
@@ -9256,13 +9256,13 @@
         <v>45917</v>
       </c>
       <c r="F210" t="n">
-        <v>0.6010204296551911</v>
+        <v>0.6325342059725293</v>
       </c>
       <c r="G210" t="n">
-        <v>0.3665107652625472</v>
+        <v>0.418813405152205</v>
       </c>
       <c r="H210" t="n">
-        <v>-0.2345096643926439</v>
+        <v>-0.2137208008203243</v>
       </c>
       <c r="I210" t="n">
         <v>5</v>
@@ -9298,13 +9298,13 @@
         <v>45917</v>
       </c>
       <c r="F211" t="n">
-        <v>0.6660903834495403</v>
+        <v>0.6969333487005431</v>
       </c>
       <c r="G211" t="n">
-        <v>0.4090646816251237</v>
+        <v>0.4709351858521071</v>
       </c>
       <c r="H211" t="n">
-        <v>-0.2570257018244166</v>
+        <v>-0.225998162848436</v>
       </c>
       <c r="I211" t="n">
         <v>5</v>
@@ -9316,7 +9316,7 @@
         <v>18</v>
       </c>
       <c r="L211" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="212">
@@ -9340,13 +9340,13 @@
         <v>45917</v>
       </c>
       <c r="F212" t="n">
-        <v>0.5975167580648931</v>
+        <v>0.6571226332772526</v>
       </c>
       <c r="G212" t="n">
-        <v>0.3583082409537519</v>
+        <v>0.4562296379001911</v>
       </c>
       <c r="H212" t="n">
-        <v>-0.2392085171111413</v>
+        <v>-0.2008929953770616</v>
       </c>
       <c r="I212" t="n">
         <v>5</v>
@@ -9382,13 +9382,13 @@
         <v>45917</v>
       </c>
       <c r="F213" t="n">
-        <v>0.5779331476714432</v>
+        <v>0.6209258083375733</v>
       </c>
       <c r="G213" t="n">
-        <v>0.3198410278407934</v>
+        <v>0.3908630226302395</v>
       </c>
       <c r="H213" t="n">
-        <v>-0.2580921198306498</v>
+        <v>-0.2300627857073338</v>
       </c>
       <c r="I213" t="n">
         <v>5</v>
@@ -9424,13 +9424,13 @@
         <v>45917</v>
       </c>
       <c r="F214" t="n">
-        <v>0.6340934735165843</v>
+        <v>0.6774640168081594</v>
       </c>
       <c r="G214" t="n">
-        <v>0.4504547228976585</v>
+        <v>0.5218881341621989</v>
       </c>
       <c r="H214" t="n">
-        <v>-0.1836387506189258</v>
+        <v>-0.1555758826459605</v>
       </c>
       <c r="I214" t="n">
         <v>5</v>
@@ -9442,7 +9442,7 @@
         <v>13</v>
       </c>
       <c r="L214" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="215">
@@ -9466,13 +9466,13 @@
         <v>45917</v>
       </c>
       <c r="F215" t="n">
-        <v>0.603225791927036</v>
+        <v>0.6404276501051219</v>
       </c>
       <c r="G215" t="n">
-        <v>0.3976968342673812</v>
+        <v>0.4579291471969623</v>
       </c>
       <c r="H215" t="n">
-        <v>-0.2055289576596547</v>
+        <v>-0.1824985029081596</v>
       </c>
       <c r="I215" t="n">
         <v>5</v>
@@ -9508,13 +9508,13 @@
         <v>45917</v>
       </c>
       <c r="F216" t="n">
-        <v>0.6398864624575893</v>
+        <v>0.6970285557319411</v>
       </c>
       <c r="G216" t="n">
-        <v>0.3899079231749679</v>
+        <v>0.4909529363173215</v>
       </c>
       <c r="H216" t="n">
-        <v>-0.2499785392826214</v>
+        <v>-0.2060756194146196</v>
       </c>
       <c r="I216" t="n">
         <v>5</v>
@@ -9550,13 +9550,13 @@
         <v>45917</v>
       </c>
       <c r="F217" t="n">
-        <v>0.571806208482407</v>
+        <v>0.6154403135130143</v>
       </c>
       <c r="G217" t="n">
-        <v>0.350943026946727</v>
+        <v>0.4183012669250833</v>
       </c>
       <c r="H217" t="n">
-        <v>-0.2208631815356801</v>
+        <v>-0.197139046587931</v>
       </c>
       <c r="I217" t="n">
         <v>5</v>
@@ -9592,13 +9592,13 @@
         <v>45917</v>
       </c>
       <c r="F218" t="n">
-        <v>0.6260699467157639</v>
+        <v>0.6625080264942051</v>
       </c>
       <c r="G218" t="n">
-        <v>0.4039717799102483</v>
+        <v>0.4682951351871608</v>
       </c>
       <c r="H218" t="n">
-        <v>-0.2220981668055156</v>
+        <v>-0.1942128913070444</v>
       </c>
       <c r="I218" t="n">
         <v>5</v>
@@ -9610,7 +9610,7 @@
         <v>17</v>
       </c>
       <c r="L218" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="219">
@@ -9634,13 +9634,13 @@
         <v>45917</v>
       </c>
       <c r="F219" t="n">
-        <v>0.6466891954088431</v>
+        <v>0.6884963133472601</v>
       </c>
       <c r="G219" t="n">
-        <v>0.439428634965135</v>
+        <v>0.5076065683176445</v>
       </c>
       <c r="H219" t="n">
-        <v>-0.2072605604437081</v>
+        <v>-0.1808897450296156</v>
       </c>
       <c r="I219" t="n">
         <v>5</v>
@@ -9676,13 +9676,13 @@
         <v>45917</v>
       </c>
       <c r="F220" t="n">
-        <v>0.5902958128041752</v>
+        <v>0.6249831779627801</v>
       </c>
       <c r="G220" t="n">
-        <v>0.3540510346861013</v>
+        <v>0.4068513035608372</v>
       </c>
       <c r="H220" t="n">
-        <v>-0.2362447781180739</v>
+        <v>-0.2181318744019429</v>
       </c>
       <c r="I220" t="n">
         <v>5</v>
@@ -9694,7 +9694,7 @@
         <v>22</v>
       </c>
       <c r="L220" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="221">
@@ -9718,13 +9718,13 @@
         <v>45917</v>
       </c>
       <c r="F221" t="n">
-        <v>0.6183454157765008</v>
+        <v>0.6501017621008514</v>
       </c>
       <c r="G221" t="n">
-        <v>0.4220616667808073</v>
+        <v>0.4719156427882325</v>
       </c>
       <c r="H221" t="n">
-        <v>-0.1962837489956936</v>
+        <v>-0.1781861193126189</v>
       </c>
       <c r="I221" t="n">
         <v>5</v>
@@ -9760,13 +9760,13 @@
         <v>45917</v>
       </c>
       <c r="F222" t="n">
-        <v>0.1458422689353367</v>
+        <v>0.1458422689353363</v>
       </c>
       <c r="G222" t="n">
-        <v>0.1507031138885193</v>
+        <v>0.1507031138885196</v>
       </c>
       <c r="H222" t="n">
-        <v>0.004860844953182508</v>
+        <v>0.004860844953183285</v>
       </c>
       <c r="I222" t="n">
         <v>5</v>
@@ -9802,13 +9802,13 @@
         <v>45917</v>
       </c>
       <c r="F223" t="n">
-        <v>0.1880303475220622</v>
+        <v>0.1880303475220623</v>
       </c>
       <c r="G223" t="n">
         <v>0.1999795579054296</v>
       </c>
       <c r="H223" t="n">
-        <v>0.01194921038336735</v>
+        <v>0.01194921038336727</v>
       </c>
       <c r="I223" t="n">
         <v>5</v>
@@ -9844,13 +9844,13 @@
         <v>45917</v>
       </c>
       <c r="F224" t="n">
-        <v>0.2240290035791924</v>
+        <v>0.2240290035791926</v>
       </c>
       <c r="G224" t="n">
-        <v>0.2219390751854407</v>
+        <v>0.2219390751854409</v>
       </c>
       <c r="H224" t="n">
-        <v>-0.002089928393751744</v>
+        <v>-0.002089928393751689</v>
       </c>
       <c r="I224" t="n">
         <v>5</v>
@@ -9886,13 +9886,13 @@
         <v>45917</v>
       </c>
       <c r="F225" t="n">
-        <v>0.1407915216239945</v>
+        <v>0.1407915216239947</v>
       </c>
       <c r="G225" t="n">
-        <v>0.1359728301369797</v>
+        <v>0.1359728301369794</v>
       </c>
       <c r="H225" t="n">
-        <v>-0.00481869148701472</v>
+        <v>-0.004818691487015359</v>
       </c>
       <c r="I225" t="n">
         <v>5</v>
@@ -9928,13 +9928,13 @@
         <v>45917</v>
       </c>
       <c r="F226" t="n">
-        <v>0.1840691064426278</v>
+        <v>0.1840691064426274</v>
       </c>
       <c r="G226" t="n">
-        <v>0.1881881497977244</v>
+        <v>0.1881881497977245</v>
       </c>
       <c r="H226" t="n">
-        <v>0.004119043355096663</v>
+        <v>0.00411904335509708</v>
       </c>
       <c r="I226" t="n">
         <v>5</v>
@@ -9970,13 +9970,13 @@
         <v>45917</v>
       </c>
       <c r="F227" t="n">
-        <v>0.2765752587064276</v>
+        <v>0.2765752587064277</v>
       </c>
       <c r="G227" t="n">
-        <v>0.2953968654850195</v>
+        <v>0.2953968654850192</v>
       </c>
       <c r="H227" t="n">
-        <v>0.0188216067785919</v>
+        <v>0.01882160677859146</v>
       </c>
       <c r="I227" t="n">
         <v>5</v>
@@ -10012,13 +10012,13 @@
         <v>45917</v>
       </c>
       <c r="F228" t="n">
-        <v>0.2967389938529978</v>
+        <v>0.2967389938529967</v>
       </c>
       <c r="G228" t="n">
-        <v>0.3090700515260646</v>
+        <v>0.3090700515260645</v>
       </c>
       <c r="H228" t="n">
-        <v>0.01233105767306686</v>
+        <v>0.01233105767306775</v>
       </c>
       <c r="I228" t="n">
         <v>5</v>
@@ -10054,25 +10054,25 @@
         <v>45922</v>
       </c>
       <c r="F229" t="n">
-        <v>0.2606566802430761</v>
+        <v>0.261895231477676</v>
       </c>
       <c r="G229" t="n">
-        <v>0.2835733335685724</v>
+        <v>0.2859608514400974</v>
       </c>
       <c r="H229" t="n">
-        <v>0.02291665332549631</v>
+        <v>0.0240656199624214</v>
       </c>
       <c r="I229" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J229" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K229" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L229" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="230">
@@ -10096,13 +10096,13 @@
         <v>45917</v>
       </c>
       <c r="F230" t="n">
-        <v>0.2618510742798916</v>
+        <v>0.261851074279891</v>
       </c>
       <c r="G230" t="n">
         <v>0.2711352422900231</v>
       </c>
       <c r="H230" t="n">
-        <v>0.009284168010131433</v>
+        <v>0.009284168010132043</v>
       </c>
       <c r="I230" t="n">
         <v>5</v>
@@ -10138,25 +10138,25 @@
         <v>45922</v>
       </c>
       <c r="F231" t="n">
-        <v>0.2586257447392735</v>
+        <v>0.2580114092997339</v>
       </c>
       <c r="G231" t="n">
-        <v>0.2753933638110052</v>
+        <v>0.277182661173053</v>
       </c>
       <c r="H231" t="n">
-        <v>0.01676761907173169</v>
+        <v>0.01917125187331903</v>
       </c>
       <c r="I231" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J231" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K231" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L231" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="232">
@@ -10180,13 +10180,13 @@
         <v>45917</v>
       </c>
       <c r="F232" t="n">
-        <v>0.2697803886132871</v>
+        <v>0.2697803886132875</v>
       </c>
       <c r="G232" t="n">
-        <v>0.2868310090474704</v>
+        <v>0.2868310090474699</v>
       </c>
       <c r="H232" t="n">
-        <v>0.01705062043418332</v>
+        <v>0.01705062043418243</v>
       </c>
       <c r="I232" t="n">
         <v>5</v>
@@ -10225,10 +10225,10 @@
         <v>0.2621209748716927</v>
       </c>
       <c r="G233" t="n">
-        <v>0.2914564482555458</v>
+        <v>0.2914564482555462</v>
       </c>
       <c r="H233" t="n">
-        <v>0.02933547338385317</v>
+        <v>0.02933547338385351</v>
       </c>
       <c r="I233" t="n">
         <v>5</v>
@@ -10264,25 +10264,25 @@
         <v>45922</v>
       </c>
       <c r="F234" t="n">
-        <v>0.2369959112223974</v>
+        <v>0.2364924299877019</v>
       </c>
       <c r="G234" t="n">
-        <v>0.2610596153018325</v>
+        <v>0.2624222984688462</v>
       </c>
       <c r="H234" t="n">
-        <v>0.02406370407943503</v>
+        <v>0.02592986848114431</v>
       </c>
       <c r="I234" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J234" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K234" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L234" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="235">
@@ -10306,13 +10306,13 @@
         <v>45917</v>
       </c>
       <c r="F235" t="n">
-        <v>0.2417587201296576</v>
+        <v>0.2417587201296573</v>
       </c>
       <c r="G235" t="n">
-        <v>0.2645274746556002</v>
+        <v>0.2645274746556003</v>
       </c>
       <c r="H235" t="n">
-        <v>0.02276875452594265</v>
+        <v>0.02276875452594307</v>
       </c>
       <c r="I235" t="n">
         <v>5</v>
@@ -10348,13 +10348,13 @@
         <v>45917</v>
       </c>
       <c r="F236" t="n">
-        <v>0.2269762273671933</v>
+        <v>0.2269762273671939</v>
       </c>
       <c r="G236" t="n">
-        <v>0.221788146924141</v>
+        <v>0.2217881469241409</v>
       </c>
       <c r="H236" t="n">
-        <v>-0.005188080443052356</v>
+        <v>-0.005188080443053023</v>
       </c>
       <c r="I236" t="n">
         <v>5</v>
@@ -10390,13 +10390,13 @@
         <v>45917</v>
       </c>
       <c r="F237" t="n">
-        <v>0.1928092132213035</v>
+        <v>0.1928092132213037</v>
       </c>
       <c r="G237" t="n">
-        <v>0.1883467076683691</v>
+        <v>0.1883467076683692</v>
       </c>
       <c r="H237" t="n">
-        <v>-0.00446250555293437</v>
+        <v>-0.004462505552934537</v>
       </c>
       <c r="I237" t="n">
         <v>5</v>
@@ -10432,13 +10432,13 @@
         <v>45917</v>
       </c>
       <c r="F238" t="n">
-        <v>0.2506949990244342</v>
+        <v>0.2506949990244339</v>
       </c>
       <c r="G238" t="n">
-        <v>0.2644212293301801</v>
+        <v>0.2644212293301799</v>
       </c>
       <c r="H238" t="n">
-        <v>0.01372623030574599</v>
+        <v>0.01372623030574605</v>
       </c>
       <c r="I238" t="n">
         <v>5</v>
@@ -10474,13 +10474,13 @@
         <v>45917</v>
       </c>
       <c r="F239" t="n">
-        <v>0.2303777307807974</v>
+        <v>0.2303777307807972</v>
       </c>
       <c r="G239" t="n">
-        <v>0.2414058051364791</v>
+        <v>0.2414058051364799</v>
       </c>
       <c r="H239" t="n">
-        <v>0.01102807435568171</v>
+        <v>0.01102807435568276</v>
       </c>
       <c r="I239" t="n">
         <v>5</v>
@@ -10516,13 +10516,13 @@
         <v>45917</v>
       </c>
       <c r="F240" t="n">
-        <v>0.2639242337501438</v>
+        <v>0.2639242337501435</v>
       </c>
       <c r="G240" t="n">
-        <v>0.2713106523313577</v>
+        <v>0.2713744056708153</v>
       </c>
       <c r="H240" t="n">
-        <v>0.007386418581213861</v>
+        <v>0.007450171920671878</v>
       </c>
       <c r="I240" t="n">
         <v>5</v>
@@ -10534,7 +10534,7 @@
         <v>30</v>
       </c>
       <c r="L240" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="241">
@@ -10558,13 +10558,13 @@
         <v>45917</v>
       </c>
       <c r="F241" t="n">
-        <v>0.2579407362652242</v>
+        <v>0.2579407362652261</v>
       </c>
       <c r="G241" t="n">
-        <v>0.2628778937457319</v>
+        <v>0.2628778937457328</v>
       </c>
       <c r="H241" t="n">
-        <v>0.004937157480507715</v>
+        <v>0.004937157480506771</v>
       </c>
       <c r="I241" t="n">
         <v>5</v>
@@ -10600,13 +10600,13 @@
         <v>45917</v>
       </c>
       <c r="F242" t="n">
-        <v>0.2767173973707341</v>
+        <v>0.2767173973707351</v>
       </c>
       <c r="G242" t="n">
-        <v>0.2777460109471916</v>
+        <v>0.2767509025656557</v>
       </c>
       <c r="H242" t="n">
-        <v>0.001028613576457504</v>
+        <v>3.350519492062443e-05</v>
       </c>
       <c r="I242" t="n">
         <v>5</v>
@@ -10618,7 +10618,7 @@
         <v>19</v>
       </c>
       <c r="L242" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="243">
@@ -10642,13 +10642,13 @@
         <v>45917</v>
       </c>
       <c r="F243" t="n">
-        <v>0.2362506532970993</v>
+        <v>0.2362506532970992</v>
       </c>
       <c r="G243" t="n">
-        <v>0.2523490047457299</v>
+        <v>0.2523490047457297</v>
       </c>
       <c r="H243" t="n">
-        <v>0.01609835144863064</v>
+        <v>0.01609835144863048</v>
       </c>
       <c r="I243" t="n">
         <v>5</v>
@@ -10684,13 +10684,13 @@
         <v>45917</v>
       </c>
       <c r="F244" t="n">
-        <v>0.2702920726463517</v>
+        <v>0.2702920726463518</v>
       </c>
       <c r="G244" t="n">
-        <v>0.2740775184030964</v>
+        <v>0.2738799269176603</v>
       </c>
       <c r="H244" t="n">
-        <v>0.00378544575674461</v>
+        <v>0.003587854271308477</v>
       </c>
       <c r="I244" t="n">
         <v>5</v>
@@ -10702,7 +10702,7 @@
         <v>18</v>
       </c>
       <c r="L244" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="245">
@@ -10726,25 +10726,25 @@
         <v>45922</v>
       </c>
       <c r="F245" t="n">
-        <v>0.2614293862863594</v>
+        <v>0.2620852231659011</v>
       </c>
       <c r="G245" t="n">
-        <v>0.2623285521540443</v>
+        <v>0.2734063697583565</v>
       </c>
       <c r="H245" t="n">
-        <v>0.000899165867684848</v>
+        <v>0.01132114659245542</v>
       </c>
       <c r="I245" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J245" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K245" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L245" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="246">
@@ -10768,10 +10768,10 @@
         <v>45917</v>
       </c>
       <c r="F246" t="n">
-        <v>0.2981893787451964</v>
+        <v>0.2981893787451968</v>
       </c>
       <c r="G246" t="n">
-        <v>0.3085926217828995</v>
+        <v>0.3085926217828999</v>
       </c>
       <c r="H246" t="n">
         <v>0.01040324303770312</v>
@@ -10810,10 +10810,10 @@
         <v>45917</v>
       </c>
       <c r="F247" t="n">
-        <v>0.2977732982923539</v>
+        <v>0.2977732982923541</v>
       </c>
       <c r="G247" t="n">
-        <v>0.3046575678709836</v>
+        <v>0.3046575678709837</v>
       </c>
       <c r="H247" t="n">
         <v>0.006884269578629643</v>
@@ -10852,13 +10852,13 @@
         <v>45917</v>
       </c>
       <c r="F248" t="n">
-        <v>0.3059389648896407</v>
+        <v>0.3059389648896408</v>
       </c>
       <c r="G248" t="n">
-        <v>0.3022140380668598</v>
+        <v>0.3022140380668594</v>
       </c>
       <c r="H248" t="n">
-        <v>-0.003724926822780861</v>
+        <v>-0.003724926822781416</v>
       </c>
       <c r="I248" t="n">
         <v>5</v>
@@ -10894,25 +10894,25 @@
         <v>45922</v>
       </c>
       <c r="F249" t="n">
-        <v>0.2970513203936218</v>
+        <v>0.2970303699474752</v>
       </c>
       <c r="G249" t="n">
-        <v>0.310054391585973</v>
+        <v>0.3055879859386098</v>
       </c>
       <c r="H249" t="n">
-        <v>0.01300307119235128</v>
+        <v>0.008557615991134637</v>
       </c>
       <c r="I249" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J249" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K249" t="n">
+        <v>7</v>
+      </c>
+      <c r="L249" t="n">
         <v>6</v>
-      </c>
-      <c r="L249" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="250">
@@ -10936,13 +10936,13 @@
         <v>45917</v>
       </c>
       <c r="F250" t="n">
-        <v>0.2531264355282876</v>
+        <v>0.2531264355282875</v>
       </c>
       <c r="G250" t="n">
         <v>0.2446452236379321</v>
       </c>
       <c r="H250" t="n">
-        <v>-0.008481211890355472</v>
+        <v>-0.008481211890355389</v>
       </c>
       <c r="I250" t="n">
         <v>5</v>
@@ -10978,13 +10978,13 @@
         <v>45917</v>
       </c>
       <c r="F251" t="n">
-        <v>0.2242210917118176</v>
+        <v>0.224221091711818</v>
       </c>
       <c r="G251" t="n">
-        <v>0.2079609791844725</v>
+        <v>0.2079609791844722</v>
       </c>
       <c r="H251" t="n">
-        <v>-0.01626011252734505</v>
+        <v>-0.01626011252734588</v>
       </c>
       <c r="I251" t="n">
         <v>5</v>
@@ -11020,13 +11020,13 @@
         <v>45917</v>
       </c>
       <c r="F252" t="n">
-        <v>0.29258333452566</v>
+        <v>0.2925833345256598</v>
       </c>
       <c r="G252" t="n">
-        <v>0.3014781066855779</v>
+        <v>0.3014781066855777</v>
       </c>
       <c r="H252" t="n">
-        <v>0.008894772159917852</v>
+        <v>0.008894772159917963</v>
       </c>
       <c r="I252" t="n">
         <v>5</v>
@@ -11062,25 +11062,25 @@
         <v>45922</v>
       </c>
       <c r="F253" t="n">
-        <v>0.3089897548970037</v>
+        <v>0.3088243715487994</v>
       </c>
       <c r="G253" t="n">
-        <v>0.3439833302420794</v>
+        <v>0.3410318789332486</v>
       </c>
       <c r="H253" t="n">
-        <v>0.03499357534507569</v>
+        <v>0.03220750738444916</v>
       </c>
       <c r="I253" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J253" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K253" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L253" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="254">
@@ -11104,13 +11104,13 @@
         <v>45917</v>
       </c>
       <c r="F254" t="n">
-        <v>0.29945153208492</v>
+        <v>0.2994515320849201</v>
       </c>
       <c r="G254" t="n">
-        <v>0.3057211120615638</v>
+        <v>0.3057211120615637</v>
       </c>
       <c r="H254" t="n">
-        <v>0.006269579976643791</v>
+        <v>0.006269579976643513</v>
       </c>
       <c r="I254" t="n">
         <v>5</v>
@@ -11146,13 +11146,13 @@
         <v>45917</v>
       </c>
       <c r="F255" t="n">
-        <v>0.3331786204944298</v>
+        <v>0.33317862049443</v>
       </c>
       <c r="G255" t="n">
-        <v>0.3541497652135571</v>
+        <v>0.3541497652135569</v>
       </c>
       <c r="H255" t="n">
-        <v>0.02097114471912737</v>
+        <v>0.02097114471912692</v>
       </c>
       <c r="I255" t="n">
         <v>5</v>
@@ -11188,25 +11188,25 @@
         <v>45922</v>
       </c>
       <c r="F256" t="n">
-        <v>0.2784490953378195</v>
+        <v>0.2785563740601013</v>
       </c>
       <c r="G256" t="n">
-        <v>0.3088923234352193</v>
+        <v>0.3102536274290981</v>
       </c>
       <c r="H256" t="n">
-        <v>0.0304432280973998</v>
+        <v>0.03169725336899676</v>
       </c>
       <c r="I256" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J256" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K256" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L256" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="257">
@@ -11230,13 +11230,13 @@
         <v>45917</v>
       </c>
       <c r="F257" t="n">
-        <v>0.3300008017870922</v>
+        <v>0.3300008017870919</v>
       </c>
       <c r="G257" t="n">
         <v>0.3356601550960443</v>
       </c>
       <c r="H257" t="n">
-        <v>0.00565935330895212</v>
+        <v>0.005659353308952397</v>
       </c>
       <c r="I257" t="n">
         <v>5</v>
@@ -11278,7 +11278,7 @@
         <v>0.2503568961044019</v>
       </c>
       <c r="H258" t="n">
-        <v>0.003940157576084763</v>
+        <v>0.00394015757608468</v>
       </c>
       <c r="I258" t="n">
         <v>5</v>
@@ -11317,10 +11317,10 @@
         <v>0.2592736434370876</v>
       </c>
       <c r="G259" t="n">
-        <v>0.2631786361046013</v>
+        <v>0.2627080662722916</v>
       </c>
       <c r="H259" t="n">
-        <v>0.003904992667513707</v>
+        <v>0.003434422835203954</v>
       </c>
       <c r="I259" t="n">
         <v>5</v>
@@ -11332,7 +11332,7 @@
         <v>18</v>
       </c>
       <c r="L259" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="260">
@@ -11356,13 +11356,13 @@
         <v>45917</v>
       </c>
       <c r="F260" t="n">
-        <v>0.2932577338293339</v>
+        <v>0.2932577338293336</v>
       </c>
       <c r="G260" t="n">
-        <v>0.3149946390332656</v>
+        <v>0.314994639033265</v>
       </c>
       <c r="H260" t="n">
-        <v>0.02173690520393168</v>
+        <v>0.0217369052039314</v>
       </c>
       <c r="I260" t="n">
         <v>5</v>
@@ -11398,13 +11398,13 @@
         <v>45917</v>
       </c>
       <c r="F261" t="n">
-        <v>0.2377412160876543</v>
+        <v>0.2377412160876539</v>
       </c>
       <c r="G261" t="n">
-        <v>0.2595386002563753</v>
+        <v>0.2595386002563755</v>
       </c>
       <c r="H261" t="n">
-        <v>0.02179738416872101</v>
+        <v>0.02179738416872165</v>
       </c>
       <c r="I261" t="n">
         <v>5</v>
@@ -11440,13 +11440,13 @@
         <v>45917</v>
       </c>
       <c r="F262" t="n">
-        <v>0.2441339029386105</v>
+        <v>0.2441339029386108</v>
       </c>
       <c r="G262" t="n">
-        <v>0.2588866944666777</v>
+        <v>0.2593366312356813</v>
       </c>
       <c r="H262" t="n">
-        <v>0.01475279152806719</v>
+        <v>0.01520272829707048</v>
       </c>
       <c r="I262" t="n">
         <v>5</v>
@@ -11458,7 +11458,7 @@
         <v>25</v>
       </c>
       <c r="L262" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="263">
@@ -11482,13 +11482,13 @@
         <v>45917</v>
       </c>
       <c r="F263" t="n">
-        <v>0.2459835086174607</v>
+        <v>0.2459835086174601</v>
       </c>
       <c r="G263" t="n">
-        <v>0.2527060259894836</v>
+        <v>0.2526623559242195</v>
       </c>
       <c r="H263" t="n">
-        <v>0.006722517372022896</v>
+        <v>0.006678847306759411</v>
       </c>
       <c r="I263" t="n">
         <v>5</v>
@@ -11500,7 +11500,7 @@
         <v>12</v>
       </c>
       <c r="L263" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="264">
@@ -11524,13 +11524,13 @@
         <v>45917</v>
       </c>
       <c r="F264" t="n">
-        <v>0.2887398302378515</v>
+        <v>0.2887398302378532</v>
       </c>
       <c r="G264" t="n">
-        <v>0.2877058869421324</v>
+        <v>0.2877058869421327</v>
       </c>
       <c r="H264" t="n">
-        <v>-0.001033943295719042</v>
+        <v>-0.001033943295720485</v>
       </c>
       <c r="I264" t="n">
         <v>5</v>
@@ -11566,13 +11566,13 @@
         <v>45917</v>
       </c>
       <c r="F265" t="n">
-        <v>0.2694421400977084</v>
+        <v>0.2694421400977087</v>
       </c>
       <c r="G265" t="n">
-        <v>0.2797463226200677</v>
+        <v>0.2797463226200674</v>
       </c>
       <c r="H265" t="n">
-        <v>0.01030418252235921</v>
+        <v>0.01030418252235871</v>
       </c>
       <c r="I265" t="n">
         <v>5</v>
@@ -11608,13 +11608,13 @@
         <v>45917</v>
       </c>
       <c r="F266" t="n">
-        <v>0.2976041118629885</v>
+        <v>0.2976041118629884</v>
       </c>
       <c r="G266" t="n">
-        <v>0.3258859915465456</v>
+        <v>0.3258426763814535</v>
       </c>
       <c r="H266" t="n">
-        <v>0.02828187968355711</v>
+        <v>0.02823856451846513</v>
       </c>
       <c r="I266" t="n">
         <v>5</v>
@@ -11626,7 +11626,7 @@
         <v>18</v>
       </c>
       <c r="L266" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="267">
@@ -11653,10 +11653,10 @@
         <v>0.3368317331662626</v>
       </c>
       <c r="G267" t="n">
-        <v>0.3573643462502682</v>
+        <v>0.3573643462502684</v>
       </c>
       <c r="H267" t="n">
-        <v>0.02053261308400567</v>
+        <v>0.02053261308400578</v>
       </c>
       <c r="I267" t="n">
         <v>5</v>
@@ -11692,13 +11692,13 @@
         <v>45917</v>
       </c>
       <c r="F268" t="n">
-        <v>0.3022220189830319</v>
+        <v>0.3022220189830321</v>
       </c>
       <c r="G268" t="n">
-        <v>0.3201162229651077</v>
+        <v>0.3201162229651079</v>
       </c>
       <c r="H268" t="n">
-        <v>0.01789420398207575</v>
+        <v>0.01789420398207581</v>
       </c>
       <c r="I268" t="n">
         <v>5</v>
@@ -11737,10 +11737,10 @@
         <v>0.2467447197992626</v>
       </c>
       <c r="G269" t="n">
-        <v>0.2475296950707059</v>
+        <v>0.2471791327276641</v>
       </c>
       <c r="H269" t="n">
-        <v>0.0007849752714433333</v>
+        <v>0.0004344129284014897</v>
       </c>
       <c r="I269" t="n">
         <v>5</v>
@@ -11752,7 +11752,7 @@
         <v>13</v>
       </c>
       <c r="L269" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="270">
@@ -11776,13 +11776,13 @@
         <v>45917</v>
       </c>
       <c r="F270" t="n">
-        <v>0.2569413439084687</v>
+        <v>0.2569413439084689</v>
       </c>
       <c r="G270" t="n">
-        <v>0.2390188024544619</v>
+        <v>0.2390188024544621</v>
       </c>
       <c r="H270" t="n">
-        <v>-0.01792254145400679</v>
+        <v>-0.01792254145400676</v>
       </c>
       <c r="I270" t="n">
         <v>5</v>
@@ -11818,13 +11818,13 @@
         <v>45917</v>
       </c>
       <c r="F271" t="n">
-        <v>0.2192086963048659</v>
+        <v>0.2192086963048661</v>
       </c>
       <c r="G271" t="n">
-        <v>0.2283250236203755</v>
+        <v>0.2283250236203758</v>
       </c>
       <c r="H271" t="n">
-        <v>0.009116327315509543</v>
+        <v>0.009116327315509654</v>
       </c>
       <c r="I271" t="n">
         <v>5</v>
@@ -11860,13 +11860,13 @@
         <v>45917</v>
       </c>
       <c r="F272" t="n">
-        <v>0.1748096093303624</v>
+        <v>0.1748096093303632</v>
       </c>
       <c r="G272" t="n">
-        <v>0.1762233934854912</v>
+        <v>0.1762233934854906</v>
       </c>
       <c r="H272" t="n">
-        <v>0.0014137841551288</v>
+        <v>0.001413784155127357</v>
       </c>
       <c r="I272" t="n">
         <v>5</v>
@@ -11902,13 +11902,13 @@
         <v>45917</v>
       </c>
       <c r="F273" t="n">
-        <v>0.2431940408160648</v>
+        <v>0.2431940408160646</v>
       </c>
       <c r="G273" t="n">
-        <v>0.235986180242379</v>
+        <v>0.2364675677665549</v>
       </c>
       <c r="H273" t="n">
-        <v>-0.007207860573685804</v>
+        <v>-0.006726473049509685</v>
       </c>
       <c r="I273" t="n">
         <v>5</v>
@@ -11920,7 +11920,7 @@
         <v>17</v>
       </c>
       <c r="L273" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="274">
@@ -11944,13 +11944,13 @@
         <v>45917</v>
       </c>
       <c r="F274" t="n">
-        <v>0.192570193657201</v>
+        <v>0.1925701936572009</v>
       </c>
       <c r="G274" t="n">
-        <v>0.2052225964535169</v>
+        <v>0.2052225964535165</v>
       </c>
       <c r="H274" t="n">
-        <v>0.01265240279631585</v>
+        <v>0.0126524027963156</v>
       </c>
       <c r="I274" t="n">
         <v>5</v>
@@ -11986,13 +11986,13 @@
         <v>45917</v>
       </c>
       <c r="F275" t="n">
-        <v>0.2078431146125492</v>
+        <v>0.207843114612549</v>
       </c>
       <c r="G275" t="n">
-        <v>0.2262092045732868</v>
+        <v>0.2262872051090691</v>
       </c>
       <c r="H275" t="n">
-        <v>0.0183660899607376</v>
+        <v>0.01844409049652004</v>
       </c>
       <c r="I275" t="n">
         <v>5</v>
@@ -12004,7 +12004,7 @@
         <v>22</v>
       </c>
       <c r="L275" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="276">
@@ -12028,13 +12028,13 @@
         <v>45917</v>
       </c>
       <c r="F276" t="n">
-        <v>0.2763860001150545</v>
+        <v>0.2763860001150547</v>
       </c>
       <c r="G276" t="n">
-        <v>0.2937360369949688</v>
+        <v>0.2937360369949686</v>
       </c>
       <c r="H276" t="n">
-        <v>0.01735003687991421</v>
+        <v>0.01735003687991393</v>
       </c>
       <c r="I276" t="n">
         <v>5</v>
@@ -12364,25 +12364,25 @@
         <v>45922</v>
       </c>
       <c r="F284" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="G284" t="n">
         <v>1</v>
       </c>
       <c r="H284" t="n">
-        <v>0</v>
+        <v>0.05555555555555558</v>
       </c>
       <c r="I284" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J284" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K284" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="L284" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="285">
@@ -12448,25 +12448,25 @@
         <v>45922</v>
       </c>
       <c r="F286" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="G286" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="H286" t="n">
-        <v>-0.25</v>
+        <v>-0.4444444444444444</v>
       </c>
       <c r="I286" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J286" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K286" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L286" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="287">
@@ -12574,25 +12574,25 @@
         <v>45922</v>
       </c>
       <c r="F289" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="G289" t="n">
-        <v>1.166666666666667</v>
+        <v>1.111111111111111</v>
       </c>
       <c r="H289" t="n">
-        <v>0.8333333333333335</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="I289" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J289" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K289" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L289" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="290">
@@ -13039,19 +13039,19 @@
         <v>0.5</v>
       </c>
       <c r="G300" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="H300" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I300" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J300" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K300" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L300" t="n">
         <v>3</v>
@@ -13204,19 +13204,19 @@
         <v>45922</v>
       </c>
       <c r="F304" t="n">
-        <v>0.5</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G304" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="H304" t="n">
-        <v>0.5</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="I304" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J304" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K304" t="n">
         <v>2</v>
@@ -13372,25 +13372,25 @@
         <v>45922</v>
       </c>
       <c r="F308" t="n">
-        <v>0.75</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G308" t="n">
         <v>0.5</v>
       </c>
       <c r="H308" t="n">
-        <v>-0.25</v>
+        <v>-0.3333333333333334</v>
       </c>
       <c r="I308" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J308" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K308" t="n">
+        <v>5</v>
+      </c>
+      <c r="L308" t="n">
         <v>3</v>
-      </c>
-      <c r="L308" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="309">
@@ -13501,16 +13501,16 @@
         <v>0</v>
       </c>
       <c r="G311" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="H311" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I311" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J311" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K311" t="n">
         <v>0</v>
@@ -14635,10 +14635,10 @@
         <v>3887.006363636363</v>
       </c>
       <c r="G338" t="n">
-        <v>7120.065384615384</v>
+        <v>7120.065384615385</v>
       </c>
       <c r="H338" t="n">
-        <v>3233.05902097902</v>
+        <v>3233.059020979022</v>
       </c>
       <c r="I338" t="n">
         <v>5</v>
@@ -14674,25 +14674,25 @@
         <v>45922</v>
       </c>
       <c r="F339" t="n">
-        <v>7958.853333333333</v>
+        <v>7780.667647058824</v>
       </c>
       <c r="G339" t="n">
-        <v>4979.483333333333</v>
+        <v>4930.302222222223</v>
       </c>
       <c r="H339" t="n">
-        <v>-2979.370000000001</v>
+        <v>-2850.365424836601</v>
       </c>
       <c r="I339" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J339" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K339" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="L339" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="340">
@@ -14758,25 +14758,25 @@
         <v>45922</v>
       </c>
       <c r="F341" t="n">
-        <v>8731.51</v>
+        <v>7548.372352941176</v>
       </c>
       <c r="G341" t="n">
-        <v>5335.62375</v>
+        <v>4935.502222222221</v>
       </c>
       <c r="H341" t="n">
-        <v>-3395.88625</v>
+        <v>-2612.870130718955</v>
       </c>
       <c r="I341" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J341" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K341" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L341" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="342">
@@ -14884,25 +14884,25 @@
         <v>45922</v>
       </c>
       <c r="F344" t="n">
-        <v>5251.395</v>
+        <v>5489.3525</v>
       </c>
       <c r="G344" t="n">
-        <v>6154.665714285714</v>
+        <v>5388.408</v>
       </c>
       <c r="H344" t="n">
-        <v>903.2707142857134</v>
+        <v>-100.9444999999996</v>
       </c>
       <c r="I344" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J344" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K344" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L344" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="345">
@@ -15139,10 +15139,10 @@
         <v>5041.224285714286</v>
       </c>
       <c r="G350" t="n">
-        <v>8110.764999999999</v>
+        <v>8110.765000000001</v>
       </c>
       <c r="H350" t="n">
-        <v>3069.540714285714</v>
+        <v>3069.540714285715</v>
       </c>
       <c r="I350" t="n">
         <v>5</v>
@@ -15181,7 +15181,7 @@
         <v>8137.931</v>
       </c>
       <c r="G351" t="n">
-        <v>5021.217096774193</v>
+        <v>5021.217096774194</v>
       </c>
       <c r="H351" t="n">
         <v>-3116.713903225806</v>
@@ -15346,22 +15346,22 @@
         <v>45922</v>
       </c>
       <c r="F355" t="n">
-        <v>3942.595</v>
+        <v>4096.143333333333</v>
       </c>
       <c r="G355" t="n">
         <v>15220.52666666667</v>
       </c>
       <c r="H355" t="n">
-        <v>11277.93166666667</v>
+        <v>11124.38333333333</v>
       </c>
       <c r="I355" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J355" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K355" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L355" t="n">
         <v>3</v>
@@ -15472,13 +15472,13 @@
         <v>45917</v>
       </c>
       <c r="F358" t="n">
-        <v>6749.483749999999</v>
+        <v>6749.48375</v>
       </c>
       <c r="G358" t="n">
         <v>10150</v>
       </c>
       <c r="H358" t="n">
-        <v>3400.516250000001</v>
+        <v>3400.51625</v>
       </c>
       <c r="I358" t="n">
         <v>5</v>
@@ -15523,10 +15523,10 @@
         <v>2456.025000000001</v>
       </c>
       <c r="I359" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J359" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K359" t="n">
         <v>2</v>
@@ -15682,25 +15682,25 @@
         <v>45922</v>
       </c>
       <c r="F363" t="n">
-        <v>9605.68</v>
+        <v>8338.628000000001</v>
       </c>
       <c r="G363" t="n">
-        <v>4645.21</v>
+        <v>7430.139999999999</v>
       </c>
       <c r="H363" t="n">
-        <v>-4960.47</v>
+        <v>-908.4880000000012</v>
       </c>
       <c r="I363" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J363" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K363" t="n">
+        <v>5</v>
+      </c>
+      <c r="L363" t="n">
         <v>3</v>
-      </c>
-      <c r="L363" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="364">
@@ -15724,13 +15724,13 @@
         <v>45917</v>
       </c>
       <c r="F364" t="n">
-        <v>8070.015</v>
+        <v>8070.014999999999</v>
       </c>
       <c r="G364" t="n">
         <v>9047.258461538462</v>
       </c>
       <c r="H364" t="n">
-        <v>977.2434615384618</v>
+        <v>977.2434615384627</v>
       </c>
       <c r="I364" t="n">
         <v>5</v>
@@ -15813,10 +15813,10 @@
       </c>
       <c r="H366" t="inlineStr"/>
       <c r="I366" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J366" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K366" t="n">
         <v>0</v>

</xml_diff>